<commit_message>
sette pb and ether pb
</commit_message>
<xml_diff>
--- a/gu_in/Map.edf/Sette.xlsx
+++ b/gu_in/Map.edf/Sette.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sandi\Desktop\Parser_1.0.2\Database\gu_in\Map.edf\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project RF X\Parser_Public_Releases\Parser_1.0.2\database\gu_in\Map.edf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E42F3C7-8C93-44E4-B156-00E7F51E662D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7E20926-11D6-43F5-B4ED-F7103AAD6880}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,20 @@
     <sheet name="Other Dummy" sheetId="7" r:id="rId7"/>
     <sheet name="Zones" sheetId="8" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -823,7 +836,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="943" uniqueCount="432">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="936" uniqueCount="428">
   <si>
     <t>char[32]</t>
   </si>
@@ -1957,18 +1970,6 @@
   </si>
   <si>
     <t>dmm32_0</t>
-  </si>
-  <si>
-    <t>dmm32_1</t>
-  </si>
-  <si>
-    <t>dmm32_2</t>
-  </si>
-  <si>
-    <t>dmm32_3</t>
-  </si>
-  <si>
-    <t>17E17</t>
   </si>
   <si>
     <t>sd141a3</t>
@@ -2125,7 +2126,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -2197,9 +2198,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2237,7 +2238,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2343,7 +2344,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2485,7 +2486,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2499,13 +2500,13 @@
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="19.109375" customWidth="1"/>
+    <col min="2" max="2" width="19.140625" customWidth="1"/>
     <col min="3" max="3" width="30" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2516,7 +2517,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -2524,10 +2525,10 @@
         <v>8</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -2538,7 +2539,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -2549,7 +2550,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -2560,7 +2561,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -2571,7 +2572,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -2582,7 +2583,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -2593,7 +2594,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>5</v>
       </c>
@@ -2604,7 +2605,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>5</v>
       </c>
@@ -2615,7 +2616,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>4</v>
       </c>
@@ -2626,7 +2627,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>5</v>
       </c>
@@ -2637,7 +2638,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>5</v>
       </c>
@@ -2648,7 +2649,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>5</v>
       </c>
@@ -2659,7 +2660,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>5</v>
       </c>
@@ -2670,7 +2671,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>6</v>
       </c>
@@ -2681,7 +2682,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>6</v>
       </c>
@@ -2692,7 +2693,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>5</v>
       </c>
@@ -2703,7 +2704,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>5</v>
       </c>
@@ -2714,7 +2715,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>6</v>
       </c>
@@ -2725,7 +2726,7 @@
         <v>7475</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>6</v>
       </c>
@@ -2736,7 +2737,7 @@
         <v>7474</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>6</v>
       </c>
@@ -2747,7 +2748,7 @@
         <v>100782</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>6</v>
       </c>
@@ -2758,7 +2759,7 @@
         <v>108015</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>6</v>
       </c>
@@ -2783,23 +2784,23 @@
       <selection activeCell="W18" sqref="W18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.6640625" customWidth="1"/>
-    <col min="2" max="2" width="27.6640625" customWidth="1"/>
+    <col min="1" max="1" width="25.7109375" customWidth="1"/>
+    <col min="2" max="2" width="27.7109375" customWidth="1"/>
     <col min="3" max="3" width="23" customWidth="1"/>
-    <col min="4" max="4" width="21.6640625" customWidth="1"/>
-    <col min="5" max="5" width="19.44140625" customWidth="1"/>
-    <col min="7" max="7" width="21.33203125" customWidth="1"/>
-    <col min="11" max="11" width="13.5546875" customWidth="1"/>
+    <col min="4" max="4" width="21.7109375" customWidth="1"/>
+    <col min="5" max="5" width="19.42578125" customWidth="1"/>
+    <col min="7" max="7" width="21.28515625" customWidth="1"/>
+    <col min="11" max="11" width="13.5703125" customWidth="1"/>
     <col min="12" max="12" width="12" customWidth="1"/>
     <col min="13" max="13" width="16" customWidth="1"/>
-    <col min="18" max="18" width="26.109375" customWidth="1"/>
-    <col min="20" max="20" width="14.88671875" customWidth="1"/>
+    <col min="18" max="18" width="26.140625" customWidth="1"/>
+    <col min="20" max="20" width="14.85546875" customWidth="1"/>
     <col min="22" max="22" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2885,7 +2886,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:28">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>37</v>
       </c>
@@ -2971,7 +2972,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="3" spans="1:28">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>65</v>
       </c>
@@ -2979,7 +2980,7 @@
         <v>66</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="D3" s="1">
         <v>46</v>
@@ -3057,7 +3058,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="4" spans="1:28">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>69</v>
       </c>
@@ -3065,7 +3066,7 @@
         <v>66</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="D4" s="1">
         <v>44</v>
@@ -3143,7 +3144,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="5" spans="1:28">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>71</v>
       </c>
@@ -3151,7 +3152,7 @@
         <v>66</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
       <c r="D5" s="1">
         <v>40</v>
@@ -3229,7 +3230,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="6" spans="1:28">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>73</v>
       </c>
@@ -3237,7 +3238,7 @@
         <v>66</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="D6" s="1">
         <v>13</v>
@@ -3315,7 +3316,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="7" spans="1:28">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>76</v>
       </c>
@@ -3323,7 +3324,7 @@
         <v>77</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
       <c r="D7" s="1">
         <v>0</v>
@@ -3401,7 +3402,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="8" spans="1:28">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>80</v>
       </c>
@@ -3409,7 +3410,7 @@
         <v>77</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
       <c r="D8" s="1">
         <v>0</v>
@@ -3487,7 +3488,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="9" spans="1:28">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>68</v>
       </c>
@@ -3495,7 +3496,7 @@
         <v>68</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="D9" s="1">
         <v>46</v>
@@ -3573,7 +3574,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="10" spans="1:28">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>68</v>
       </c>
@@ -3581,7 +3582,7 @@
         <v>68</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="D10" s="1">
         <v>44</v>
@@ -3659,7 +3660,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="11" spans="1:28">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>68</v>
       </c>
@@ -3667,7 +3668,7 @@
         <v>68</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="D11" s="1">
         <v>40</v>
@@ -3745,7 +3746,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="12" spans="1:28">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>68</v>
       </c>
@@ -3753,7 +3754,7 @@
         <v>68</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="D12" s="1">
         <v>0</v>
@@ -3831,7 +3832,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="13" spans="1:28">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>68</v>
       </c>
@@ -3839,7 +3840,7 @@
         <v>68</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="D13" s="1">
         <v>0</v>
@@ -3929,9 +3930,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -3957,7 +3958,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>40</v>
       </c>
@@ -3994,9 +3995,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -4013,7 +4014,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>89</v>
       </c>
@@ -4030,7 +4031,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>51</v>
       </c>
@@ -4044,10 +4045,10 @@
         <v>203</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>288</v>
       </c>
@@ -4061,10 +4062,10 @@
         <v>100</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>72</v>
       </c>
@@ -4078,10 +4079,10 @@
         <v>308</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>289</v>
       </c>
@@ -4095,10 +4096,10 @@
         <v>308</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>112</v>
       </c>
@@ -4112,10 +4113,10 @@
         <v>297</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>134</v>
       </c>
@@ -4129,10 +4130,10 @@
         <v>249</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>280</v>
       </c>
@@ -4146,10 +4147,10 @@
         <v>270</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>232</v>
       </c>
@@ -4163,7 +4164,7 @@
         <v>241</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
     </row>
   </sheetData>
@@ -4173,19 +4174,19 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:J236"/>
+  <dimension ref="A1:J233"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="A48" sqref="A48:XFD64"/>
+    <sheetView tabSelected="1" topLeftCell="A206" workbookViewId="0">
+      <selection activeCell="P231" sqref="P231"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.109375" customWidth="1"/>
-    <col min="2" max="2" width="21.44140625" customWidth="1"/>
+    <col min="1" max="1" width="19.140625" customWidth="1"/>
+    <col min="2" max="2" width="21.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -4217,7 +4218,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>96</v>
       </c>
@@ -4249,7 +4250,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>107</v>
       </c>
@@ -4263,7 +4264,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>107</v>
       </c>
@@ -4295,7 +4296,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>107</v>
       </c>
@@ -4327,7 +4328,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>107</v>
       </c>
@@ -4359,7 +4360,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>107</v>
       </c>
@@ -4391,7 +4392,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>115</v>
       </c>
@@ -4405,7 +4406,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>115</v>
       </c>
@@ -4437,7 +4438,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>115</v>
       </c>
@@ -4469,7 +4470,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>115</v>
       </c>
@@ -4501,7 +4502,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>115</v>
       </c>
@@ -4533,7 +4534,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>123</v>
       </c>
@@ -4547,7 +4548,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>123</v>
       </c>
@@ -4579,7 +4580,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>123</v>
       </c>
@@ -4611,7 +4612,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>123</v>
       </c>
@@ -4643,7 +4644,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>123</v>
       </c>
@@ -4675,7 +4676,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>128</v>
       </c>
@@ -4689,7 +4690,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:10">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>128</v>
       </c>
@@ -4721,7 +4722,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>128</v>
       </c>
@@ -4753,7 +4754,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>128</v>
       </c>
@@ -4785,7 +4786,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="22" spans="1:10">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>128</v>
       </c>
@@ -4817,7 +4818,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="23" spans="1:10">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>138</v>
       </c>
@@ -4831,7 +4832,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:10">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>138</v>
       </c>
@@ -4863,7 +4864,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="25" spans="1:10">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>138</v>
       </c>
@@ -4895,7 +4896,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="26" spans="1:10">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>138</v>
       </c>
@@ -4927,7 +4928,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="27" spans="1:10">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>138</v>
       </c>
@@ -4959,7 +4960,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="28" spans="1:10">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>144</v>
       </c>
@@ -4973,7 +4974,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:10">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>144</v>
       </c>
@@ -5005,7 +5006,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="30" spans="1:10">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>144</v>
       </c>
@@ -5037,7 +5038,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="31" spans="1:10">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>144</v>
       </c>
@@ -5069,7 +5070,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="32" spans="1:10">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>144</v>
       </c>
@@ -5101,7 +5102,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="33" spans="1:10">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>149</v>
       </c>
@@ -5115,7 +5116,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:10">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>149</v>
       </c>
@@ -5147,7 +5148,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="35" spans="1:10">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>149</v>
       </c>
@@ -5179,7 +5180,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="36" spans="1:10">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>149</v>
       </c>
@@ -5211,7 +5212,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="37" spans="1:10">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>149</v>
       </c>
@@ -5243,7 +5244,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="38" spans="1:10">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>158</v>
       </c>
@@ -5257,7 +5258,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:10">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>158</v>
       </c>
@@ -5289,7 +5290,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="40" spans="1:10">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>158</v>
       </c>
@@ -5321,7 +5322,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="41" spans="1:10">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>158</v>
       </c>
@@ -5353,7 +5354,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="42" spans="1:10">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>158</v>
       </c>
@@ -5385,7 +5386,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="43" spans="1:10">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>163</v>
       </c>
@@ -5399,7 +5400,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:10">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>163</v>
       </c>
@@ -5431,7 +5432,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="45" spans="1:10">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>163</v>
       </c>
@@ -5463,7 +5464,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="46" spans="1:10">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>163</v>
       </c>
@@ -5495,7 +5496,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="47" spans="1:10">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>163</v>
       </c>
@@ -5527,7 +5528,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="48" spans="1:10">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>169</v>
       </c>
@@ -5541,7 +5542,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:10">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>169</v>
       </c>
@@ -5573,7 +5574,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="50" spans="1:10">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>169</v>
       </c>
@@ -5605,7 +5606,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="51" spans="1:10">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>169</v>
       </c>
@@ -5637,7 +5638,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="52" spans="1:10">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>169</v>
       </c>
@@ -5669,7 +5670,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="53" spans="1:10">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>169</v>
       </c>
@@ -5701,7 +5702,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="54" spans="1:10">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>169</v>
       </c>
@@ -5733,7 +5734,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="55" spans="1:10">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>169</v>
       </c>
@@ -5765,7 +5766,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="56" spans="1:10">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>169</v>
       </c>
@@ -5797,7 +5798,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="57" spans="1:10">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>169</v>
       </c>
@@ -5829,7 +5830,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="58" spans="1:10">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>169</v>
       </c>
@@ -5861,7 +5862,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="59" spans="1:10">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>169</v>
       </c>
@@ -5893,7 +5894,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="60" spans="1:10">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>169</v>
       </c>
@@ -5925,7 +5926,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="61" spans="1:10">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>169</v>
       </c>
@@ -5957,7 +5958,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="62" spans="1:10">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>169</v>
       </c>
@@ -5989,7 +5990,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="63" spans="1:10">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>169</v>
       </c>
@@ -6021,7 +6022,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="64" spans="1:10">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>169</v>
       </c>
@@ -6053,7 +6054,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="65" spans="1:10">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>187</v>
       </c>
@@ -6067,7 +6068,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:10">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>187</v>
       </c>
@@ -6099,7 +6100,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="67" spans="1:10">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>187</v>
       </c>
@@ -6131,7 +6132,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="68" spans="1:10">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>187</v>
       </c>
@@ -6163,7 +6164,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="69" spans="1:10">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>187</v>
       </c>
@@ -6195,7 +6196,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="70" spans="1:10">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>187</v>
       </c>
@@ -6227,7 +6228,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="71" spans="1:10">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>187</v>
       </c>
@@ -6259,7 +6260,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="72" spans="1:10">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>187</v>
       </c>
@@ -6291,7 +6292,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="73" spans="1:10">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>187</v>
       </c>
@@ -6323,7 +6324,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="74" spans="1:10">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>187</v>
       </c>
@@ -6355,7 +6356,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="75" spans="1:10">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>187</v>
       </c>
@@ -6387,7 +6388,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="76" spans="1:10">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>187</v>
       </c>
@@ -6419,7 +6420,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="77" spans="1:10">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>187</v>
       </c>
@@ -6451,7 +6452,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="78" spans="1:10">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>187</v>
       </c>
@@ -6483,7 +6484,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="79" spans="1:10">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>187</v>
       </c>
@@ -6515,7 +6516,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="80" spans="1:10">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>187</v>
       </c>
@@ -6547,7 +6548,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="81" spans="1:10">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>187</v>
       </c>
@@ -6579,7 +6580,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="82" spans="1:10">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>204</v>
       </c>
@@ -6593,7 +6594,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:10">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>204</v>
       </c>
@@ -6625,7 +6626,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="84" spans="1:10">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>204</v>
       </c>
@@ -6657,7 +6658,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="85" spans="1:10">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>204</v>
       </c>
@@ -6689,7 +6690,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="86" spans="1:10">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>204</v>
       </c>
@@ -6721,7 +6722,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="87" spans="1:10">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>204</v>
       </c>
@@ -6753,7 +6754,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="88" spans="1:10">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>204</v>
       </c>
@@ -6785,7 +6786,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="89" spans="1:10">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>204</v>
       </c>
@@ -6817,7 +6818,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="90" spans="1:10">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>204</v>
       </c>
@@ -6849,7 +6850,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="91" spans="1:10">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>204</v>
       </c>
@@ -6881,7 +6882,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="92" spans="1:10">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>204</v>
       </c>
@@ -6913,7 +6914,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="93" spans="1:10">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>204</v>
       </c>
@@ -6945,7 +6946,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="94" spans="1:10">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>204</v>
       </c>
@@ -6977,7 +6978,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="95" spans="1:10">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
         <v>204</v>
       </c>
@@ -7009,7 +7010,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="96" spans="1:10">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
         <v>204</v>
       </c>
@@ -7041,7 +7042,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="97" spans="1:10">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>204</v>
       </c>
@@ -7073,7 +7074,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="98" spans="1:10">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
         <v>204</v>
       </c>
@@ -7105,7 +7106,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="99" spans="1:10">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
         <v>221</v>
       </c>
@@ -7119,7 +7120,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:10">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
         <v>221</v>
       </c>
@@ -7151,7 +7152,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="101" spans="1:10">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
         <v>221</v>
       </c>
@@ -7183,7 +7184,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="102" spans="1:10">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
         <v>221</v>
       </c>
@@ -7215,7 +7216,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="103" spans="1:10">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
         <v>221</v>
       </c>
@@ -7247,7 +7248,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="104" spans="1:10">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
         <v>221</v>
       </c>
@@ -7279,7 +7280,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="105" spans="1:10">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
         <v>221</v>
       </c>
@@ -7311,7 +7312,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="106" spans="1:10">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
         <v>221</v>
       </c>
@@ -7343,7 +7344,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="107" spans="1:10">
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
         <v>221</v>
       </c>
@@ -7375,7 +7376,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="108" spans="1:10">
+    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
         <v>221</v>
       </c>
@@ -7407,7 +7408,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="109" spans="1:10">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
         <v>221</v>
       </c>
@@ -7439,7 +7440,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="110" spans="1:10">
+    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
         <v>221</v>
       </c>
@@ -7471,7 +7472,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="111" spans="1:10">
+    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
         <v>221</v>
       </c>
@@ -7503,7 +7504,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="112" spans="1:10">
+    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
         <v>221</v>
       </c>
@@ -7535,7 +7536,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="113" spans="1:10">
+    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
         <v>221</v>
       </c>
@@ -7567,7 +7568,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="114" spans="1:10">
+    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
         <v>221</v>
       </c>
@@ -7599,7 +7600,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="115" spans="1:10">
+    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
         <v>221</v>
       </c>
@@ -7631,7 +7632,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="116" spans="1:10">
+    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
         <v>239</v>
       </c>
@@ -7645,7 +7646,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:10">
+    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
         <v>239</v>
       </c>
@@ -7677,7 +7678,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="118" spans="1:10">
+    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
         <v>239</v>
       </c>
@@ -7709,7 +7710,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="119" spans="1:10">
+    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
         <v>239</v>
       </c>
@@ -7741,7 +7742,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="120" spans="1:10">
+    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
         <v>239</v>
       </c>
@@ -7773,7 +7774,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="121" spans="1:10">
+    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
         <v>239</v>
       </c>
@@ -7805,7 +7806,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="122" spans="1:10">
+    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
         <v>239</v>
       </c>
@@ -7837,7 +7838,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="123" spans="1:10">
+    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
         <v>239</v>
       </c>
@@ -7869,7 +7870,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="124" spans="1:10">
+    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
         <v>239</v>
       </c>
@@ -7901,7 +7902,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="125" spans="1:10">
+    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
         <v>239</v>
       </c>
@@ -7933,7 +7934,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="126" spans="1:10">
+    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
         <v>239</v>
       </c>
@@ -7965,7 +7966,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="127" spans="1:10">
+    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
         <v>239</v>
       </c>
@@ -7997,7 +7998,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="128" spans="1:10">
+    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
         <v>239</v>
       </c>
@@ -8029,7 +8030,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="129" spans="1:10">
+    <row r="129" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
         <v>239</v>
       </c>
@@ -8061,7 +8062,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="130" spans="1:10">
+    <row r="130" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
         <v>239</v>
       </c>
@@ -8093,7 +8094,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="131" spans="1:10">
+    <row r="131" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
         <v>239</v>
       </c>
@@ -8125,7 +8126,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="132" spans="1:10">
+    <row r="132" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
         <v>239</v>
       </c>
@@ -8157,7 +8158,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="133" spans="1:10">
+    <row r="133" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
         <v>257</v>
       </c>
@@ -8171,7 +8172,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:10">
+    <row r="134" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
         <v>257</v>
       </c>
@@ -8203,7 +8204,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="135" spans="1:10">
+    <row r="135" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
         <v>257</v>
       </c>
@@ -8235,7 +8236,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="136" spans="1:10">
+    <row r="136" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
         <v>257</v>
       </c>
@@ -8267,7 +8268,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="137" spans="1:10">
+    <row r="137" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
         <v>257</v>
       </c>
@@ -8299,7 +8300,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="138" spans="1:10">
+    <row r="138" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A138" s="1" t="s">
         <v>257</v>
       </c>
@@ -8331,7 +8332,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="139" spans="1:10">
+    <row r="139" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A139" s="1" t="s">
         <v>257</v>
       </c>
@@ -8363,7 +8364,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="140" spans="1:10">
+    <row r="140" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
         <v>257</v>
       </c>
@@ -8395,7 +8396,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="141" spans="1:10">
+    <row r="141" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A141" s="1" t="s">
         <v>257</v>
       </c>
@@ -8427,7 +8428,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="142" spans="1:10">
+    <row r="142" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A142" s="1" t="s">
         <v>257</v>
       </c>
@@ -8459,7 +8460,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="143" spans="1:10">
+    <row r="143" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A143" s="1" t="s">
         <v>257</v>
       </c>
@@ -8491,7 +8492,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="144" spans="1:10">
+    <row r="144" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A144" s="1" t="s">
         <v>257</v>
       </c>
@@ -8523,7 +8524,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="145" spans="1:10">
+    <row r="145" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A145" s="1" t="s">
         <v>257</v>
       </c>
@@ -8555,7 +8556,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="146" spans="1:10">
+    <row r="146" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A146" s="1" t="s">
         <v>271</v>
       </c>
@@ -8569,7 +8570,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="1:10">
+    <row r="147" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A147" s="1" t="s">
         <v>271</v>
       </c>
@@ -8601,7 +8602,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="148" spans="1:10">
+    <row r="148" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A148" s="1" t="s">
         <v>271</v>
       </c>
@@ -8633,7 +8634,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="149" spans="1:10">
+    <row r="149" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A149" s="1" t="s">
         <v>271</v>
       </c>
@@ -8665,7 +8666,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="150" spans="1:10">
+    <row r="150" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A150" s="1" t="s">
         <v>271</v>
       </c>
@@ -8697,7 +8698,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="151" spans="1:10">
+    <row r="151" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A151" s="1" t="s">
         <v>280</v>
       </c>
@@ -8711,7 +8712,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" spans="1:10">
+    <row r="152" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A152" s="1" t="s">
         <v>280</v>
       </c>
@@ -8743,7 +8744,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="153" spans="1:10">
+    <row r="153" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A153" s="1" t="s">
         <v>280</v>
       </c>
@@ -8775,7 +8776,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="154" spans="1:10">
+    <row r="154" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A154" s="1" t="s">
         <v>280</v>
       </c>
@@ -8807,7 +8808,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="155" spans="1:10">
+    <row r="155" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A155" s="1" t="s">
         <v>280</v>
       </c>
@@ -8839,7 +8840,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="156" spans="1:10">
+    <row r="156" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A156" s="1" t="s">
         <v>286</v>
       </c>
@@ -8853,7 +8854,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" spans="1:10">
+    <row r="157" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A157" s="1" t="s">
         <v>286</v>
       </c>
@@ -8885,7 +8886,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="158" spans="1:10">
+    <row r="158" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A158" s="1" t="s">
         <v>286</v>
       </c>
@@ -8917,7 +8918,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="159" spans="1:10">
+    <row r="159" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A159" s="1" t="s">
         <v>286</v>
       </c>
@@ -8949,7 +8950,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="160" spans="1:10">
+    <row r="160" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A160" s="1" t="s">
         <v>286</v>
       </c>
@@ -8981,7 +8982,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="161" spans="1:10">
+    <row r="161" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A161" s="1" t="s">
         <v>291</v>
       </c>
@@ -8995,7 +8996,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="162" spans="1:10">
+    <row r="162" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A162" s="1" t="s">
         <v>291</v>
       </c>
@@ -9027,7 +9028,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="163" spans="1:10">
+    <row r="163" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A163" s="1" t="s">
         <v>291</v>
       </c>
@@ -9059,7 +9060,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="164" spans="1:10">
+    <row r="164" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A164" s="1" t="s">
         <v>291</v>
       </c>
@@ -9091,7 +9092,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="165" spans="1:10">
+    <row r="165" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A165" s="1" t="s">
         <v>291</v>
       </c>
@@ -9123,7 +9124,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="166" spans="1:10">
+    <row r="166" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A166" s="1" t="s">
         <v>299</v>
       </c>
@@ -9137,7 +9138,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="167" spans="1:10">
+    <row r="167" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A167" s="1" t="s">
         <v>299</v>
       </c>
@@ -9169,7 +9170,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="168" spans="1:10">
+    <row r="168" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A168" s="1" t="s">
         <v>299</v>
       </c>
@@ -9201,7 +9202,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="169" spans="1:10">
+    <row r="169" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A169" s="1" t="s">
         <v>299</v>
       </c>
@@ -9233,7 +9234,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="170" spans="1:10">
+    <row r="170" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A170" s="1" t="s">
         <v>299</v>
       </c>
@@ -9265,7 +9266,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="171" spans="1:10">
+    <row r="171" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A171" s="1" t="s">
         <v>304</v>
       </c>
@@ -9279,7 +9280,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="172" spans="1:10">
+    <row r="172" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A172" s="1" t="s">
         <v>304</v>
       </c>
@@ -9311,7 +9312,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="173" spans="1:10">
+    <row r="173" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A173" s="1" t="s">
         <v>304</v>
       </c>
@@ -9343,7 +9344,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="174" spans="1:10">
+    <row r="174" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A174" s="1" t="s">
         <v>304</v>
       </c>
@@ -9375,7 +9376,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="175" spans="1:10">
+    <row r="175" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A175" s="1" t="s">
         <v>304</v>
       </c>
@@ -9407,7 +9408,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="176" spans="1:10">
+    <row r="176" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A176" s="1" t="s">
         <v>309</v>
       </c>
@@ -9421,7 +9422,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="177" spans="1:10">
+    <row r="177" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A177" s="1" t="s">
         <v>309</v>
       </c>
@@ -9453,7 +9454,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="178" spans="1:10">
+    <row r="178" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A178" s="1" t="s">
         <v>309</v>
       </c>
@@ -9485,7 +9486,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="179" spans="1:10">
+    <row r="179" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A179" s="1" t="s">
         <v>309</v>
       </c>
@@ -9517,7 +9518,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="180" spans="1:10">
+    <row r="180" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A180" s="1" t="s">
         <v>309</v>
       </c>
@@ -9549,7 +9550,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="181" spans="1:10">
+    <row r="181" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A181" s="1" t="s">
         <v>318</v>
       </c>
@@ -9563,7 +9564,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="182" spans="1:10">
+    <row r="182" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A182" s="1" t="s">
         <v>318</v>
       </c>
@@ -9595,7 +9596,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="183" spans="1:10">
+    <row r="183" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A183" s="1" t="s">
         <v>318</v>
       </c>
@@ -9627,7 +9628,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="184" spans="1:10">
+    <row r="184" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A184" s="1" t="s">
         <v>318</v>
       </c>
@@ -9659,7 +9660,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="185" spans="1:10">
+    <row r="185" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A185" s="1" t="s">
         <v>318</v>
       </c>
@@ -9691,7 +9692,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="186" spans="1:10">
+    <row r="186" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A186" s="1" t="s">
         <v>318</v>
       </c>
@@ -9723,7 +9724,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="187" spans="1:10">
+    <row r="187" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A187" s="1" t="s">
         <v>318</v>
       </c>
@@ -9755,7 +9756,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="188" spans="1:10">
+    <row r="188" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A188" s="1" t="s">
         <v>318</v>
       </c>
@@ -9787,7 +9788,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="189" spans="1:10">
+    <row r="189" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A189" s="1" t="s">
         <v>318</v>
       </c>
@@ -9819,7 +9820,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="190" spans="1:10">
+    <row r="190" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A190" s="1" t="s">
         <v>328</v>
       </c>
@@ -9833,7 +9834,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="191" spans="1:10">
+    <row r="191" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A191" s="1" t="s">
         <v>328</v>
       </c>
@@ -9865,7 +9866,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="192" spans="1:10">
+    <row r="192" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A192" s="1" t="s">
         <v>328</v>
       </c>
@@ -9897,7 +9898,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="193" spans="1:10">
+    <row r="193" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A193" s="1" t="s">
         <v>328</v>
       </c>
@@ -9929,7 +9930,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="194" spans="1:10">
+    <row r="194" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A194" s="1" t="s">
         <v>328</v>
       </c>
@@ -9961,7 +9962,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="195" spans="1:10">
+    <row r="195" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A195" s="1" t="s">
         <v>328</v>
       </c>
@@ -9993,7 +9994,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="196" spans="1:10">
+    <row r="196" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A196" s="1" t="s">
         <v>328</v>
       </c>
@@ -10025,7 +10026,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="197" spans="1:10">
+    <row r="197" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A197" s="1" t="s">
         <v>328</v>
       </c>
@@ -10057,7 +10058,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="198" spans="1:10">
+    <row r="198" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A198" s="1" t="s">
         <v>328</v>
       </c>
@@ -10089,7 +10090,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="199" spans="1:10">
+    <row r="199" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A199" s="1" t="s">
         <v>328</v>
       </c>
@@ -10121,7 +10122,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="200" spans="1:10">
+    <row r="200" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A200" s="1" t="s">
         <v>328</v>
       </c>
@@ -10153,7 +10154,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="201" spans="1:10">
+    <row r="201" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A201" s="1" t="s">
         <v>328</v>
       </c>
@@ -10185,7 +10186,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="202" spans="1:10">
+    <row r="202" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A202" s="1" t="s">
         <v>328</v>
       </c>
@@ -10217,7 +10218,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="203" spans="1:10">
+    <row r="203" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A203" s="1" t="s">
         <v>328</v>
       </c>
@@ -10249,7 +10250,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="204" spans="1:10">
+    <row r="204" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A204" s="1" t="s">
         <v>328</v>
       </c>
@@ -10281,7 +10282,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="205" spans="1:10">
+    <row r="205" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A205" s="1" t="s">
         <v>328</v>
       </c>
@@ -10313,7 +10314,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="206" spans="1:10">
+    <row r="206" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A206" s="1" t="s">
         <v>328</v>
       </c>
@@ -10345,7 +10346,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="207" spans="1:10">
+    <row r="207" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A207" s="1" t="s">
         <v>346</v>
       </c>
@@ -10359,7 +10360,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="208" spans="1:10">
+    <row r="208" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A208" s="1" t="s">
         <v>346</v>
       </c>
@@ -10391,7 +10392,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="209" spans="1:10">
+    <row r="209" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A209" s="1" t="s">
         <v>346</v>
       </c>
@@ -10423,7 +10424,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="210" spans="1:10">
+    <row r="210" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A210" s="1" t="s">
         <v>346</v>
       </c>
@@ -10455,7 +10456,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="211" spans="1:10">
+    <row r="211" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A211" s="1" t="s">
         <v>346</v>
       </c>
@@ -10487,7 +10488,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="212" spans="1:10">
+    <row r="212" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A212" s="1" t="s">
         <v>352</v>
       </c>
@@ -10501,7 +10502,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="213" spans="1:10">
+    <row r="213" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A213" s="1" t="s">
         <v>352</v>
       </c>
@@ -10533,7 +10534,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="214" spans="1:10">
+    <row r="214" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A214" s="1" t="s">
         <v>352</v>
       </c>
@@ -10565,7 +10566,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="215" spans="1:10">
+    <row r="215" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A215" s="1" t="s">
         <v>352</v>
       </c>
@@ -10597,7 +10598,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="216" spans="1:10">
+    <row r="216" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A216" s="1" t="s">
         <v>352</v>
       </c>
@@ -10629,7 +10630,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="217" spans="1:10">
+    <row r="217" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A217" s="1" t="s">
         <v>358</v>
       </c>
@@ -10643,7 +10644,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="218" spans="1:10">
+    <row r="218" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A218" s="1" t="s">
         <v>358</v>
       </c>
@@ -10675,7 +10676,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="219" spans="1:10">
+    <row r="219" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A219" s="1" t="s">
         <v>358</v>
       </c>
@@ -10707,7 +10708,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="220" spans="1:10">
+    <row r="220" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A220" s="1" t="s">
         <v>358</v>
       </c>
@@ -10739,7 +10740,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="221" spans="1:10">
+    <row r="221" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A221" s="1" t="s">
         <v>358</v>
       </c>
@@ -10771,7 +10772,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="222" spans="1:10">
+    <row r="222" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A222" s="1" t="s">
         <v>364</v>
       </c>
@@ -10785,7 +10786,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="223" spans="1:10">
+    <row r="223" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A223" s="1" t="s">
         <v>364</v>
       </c>
@@ -10817,7 +10818,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="224" spans="1:10">
+    <row r="224" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A224" s="1" t="s">
         <v>364</v>
       </c>
@@ -10849,7 +10850,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="225" spans="1:10">
+    <row r="225" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A225" s="1" t="s">
         <v>364</v>
       </c>
@@ -10881,7 +10882,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="226" spans="1:10">
+    <row r="226" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A226" s="1" t="s">
         <v>364</v>
       </c>
@@ -10913,7 +10914,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="227" spans="1:10">
+    <row r="227" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A227" s="1" t="s">
         <v>370</v>
       </c>
@@ -10927,7 +10928,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="228" spans="1:10">
+    <row r="228" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A228" s="1" t="s">
         <v>370</v>
       </c>
@@ -10959,7 +10960,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="229" spans="1:10">
+    <row r="229" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A229" s="1" t="s">
         <v>370</v>
       </c>
@@ -10991,7 +10992,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="230" spans="1:10">
+    <row r="230" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A230" s="1" t="s">
         <v>370</v>
       </c>
@@ -11023,7 +11024,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="231" spans="1:10">
+    <row r="231" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A231" s="1" t="s">
         <v>370</v>
       </c>
@@ -11055,7 +11056,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="232" spans="1:10">
+    <row r="232" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A232" s="1" t="s">
         <v>376</v>
       </c>
@@ -11069,7 +11070,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="233" spans="1:10">
+    <row r="233" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A233" s="1" t="s">
         <v>376</v>
       </c>
@@ -11083,13 +11084,13 @@
         <v>0</v>
       </c>
       <c r="E233" s="1">
-        <v>-2653</v>
+        <v>0</v>
       </c>
       <c r="F233" s="1">
-        <v>-95</v>
+        <v>-110</v>
       </c>
       <c r="G233" s="1">
-        <v>2448</v>
+        <v>0</v>
       </c>
       <c r="H233" s="1">
         <v>100</v>
@@ -11098,102 +11099,6 @@
         <v>200</v>
       </c>
       <c r="J233" s="1">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="234" spans="1:10">
-      <c r="A234" s="1" t="s">
-        <v>376</v>
-      </c>
-      <c r="B234" s="1" t="s">
-        <v>378</v>
-      </c>
-      <c r="C234" s="1">
-        <v>25</v>
-      </c>
-      <c r="D234" s="1">
-        <v>0</v>
-      </c>
-      <c r="E234" s="1">
-        <v>-2553</v>
-      </c>
-      <c r="F234" s="1">
-        <v>-95</v>
-      </c>
-      <c r="G234" s="1">
-        <v>2448</v>
-      </c>
-      <c r="H234" s="1">
-        <v>100</v>
-      </c>
-      <c r="I234" s="1">
-        <v>200</v>
-      </c>
-      <c r="J234" s="1">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="235" spans="1:10">
-      <c r="A235" s="1" t="s">
-        <v>376</v>
-      </c>
-      <c r="B235" s="1" t="s">
-        <v>379</v>
-      </c>
-      <c r="C235" s="1">
-        <v>25</v>
-      </c>
-      <c r="D235" s="1">
-        <v>0</v>
-      </c>
-      <c r="E235" s="1">
-        <v>-2653</v>
-      </c>
-      <c r="F235" s="1">
-        <v>-95</v>
-      </c>
-      <c r="G235" s="1">
-        <v>2548</v>
-      </c>
-      <c r="H235" s="1">
-        <v>100</v>
-      </c>
-      <c r="I235" s="1">
-        <v>200</v>
-      </c>
-      <c r="J235" s="1">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="236" spans="1:10">
-      <c r="A236" s="1" t="s">
-        <v>376</v>
-      </c>
-      <c r="B236" s="1" t="s">
-        <v>380</v>
-      </c>
-      <c r="C236" s="1">
-        <v>25</v>
-      </c>
-      <c r="D236" s="1">
-        <v>0</v>
-      </c>
-      <c r="E236" s="1">
-        <v>-2553</v>
-      </c>
-      <c r="F236" s="1">
-        <v>-95</v>
-      </c>
-      <c r="G236" s="1">
-        <v>2548</v>
-      </c>
-      <c r="H236" s="1">
-        <v>100</v>
-      </c>
-      <c r="I236" s="1">
-        <v>200</v>
-      </c>
-      <c r="J236" s="1">
         <v>100</v>
       </c>
     </row>
@@ -11207,16 +11112,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:H83"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41:XFD41"/>
+    <sheetView topLeftCell="A63" workbookViewId="0">
+      <selection activeCell="E86" sqref="E86"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="19.33203125" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -11242,7 +11147,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>96</v>
       </c>
@@ -11268,7 +11173,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>107</v>
       </c>
@@ -11294,7 +11199,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>107</v>
       </c>
@@ -11320,7 +11225,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>107</v>
       </c>
@@ -11346,7 +11251,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>115</v>
       </c>
@@ -11372,7 +11277,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>115</v>
       </c>
@@ -11398,7 +11303,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>115</v>
       </c>
@@ -11424,7 +11329,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>115</v>
       </c>
@@ -11450,7 +11355,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>123</v>
       </c>
@@ -11476,7 +11381,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>123</v>
       </c>
@@ -11502,7 +11407,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>123</v>
       </c>
@@ -11528,7 +11433,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>123</v>
       </c>
@@ -11554,7 +11459,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>123</v>
       </c>
@@ -11580,7 +11485,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>128</v>
       </c>
@@ -11606,7 +11511,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>128</v>
       </c>
@@ -11632,7 +11537,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>128</v>
       </c>
@@ -11658,7 +11563,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>128</v>
       </c>
@@ -11684,7 +11589,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>128</v>
       </c>
@@ -11710,7 +11615,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>138</v>
       </c>
@@ -11736,7 +11641,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>138</v>
       </c>
@@ -11762,7 +11667,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>138</v>
       </c>
@@ -11788,7 +11693,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>138</v>
       </c>
@@ -11814,7 +11719,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>138</v>
       </c>
@@ -11840,7 +11745,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>144</v>
       </c>
@@ -11866,7 +11771,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>144</v>
       </c>
@@ -11892,7 +11797,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>144</v>
       </c>
@@ -11918,7 +11823,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>144</v>
       </c>
@@ -11944,7 +11849,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>149</v>
       </c>
@@ -11970,7 +11875,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>149</v>
       </c>
@@ -11996,7 +11901,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>149</v>
       </c>
@@ -12022,7 +11927,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>149</v>
       </c>
@@ -12048,7 +11953,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:8">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>158</v>
       </c>
@@ -12074,7 +11979,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>158</v>
       </c>
@@ -12100,7 +12005,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>158</v>
       </c>
@@ -12126,7 +12031,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:8">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>158</v>
       </c>
@@ -12152,7 +12057,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:8">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>163</v>
       </c>
@@ -12178,7 +12083,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:8">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>163</v>
       </c>
@@ -12204,7 +12109,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:8">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>163</v>
       </c>
@@ -12230,7 +12135,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:8">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>163</v>
       </c>
@@ -12256,7 +12161,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:8">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>169</v>
       </c>
@@ -12282,7 +12187,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:8">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>187</v>
       </c>
@@ -12308,7 +12213,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:8">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>204</v>
       </c>
@@ -12334,7 +12239,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:8">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>221</v>
       </c>
@@ -12360,7 +12265,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:8">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>239</v>
       </c>
@@ -12386,7 +12291,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:8">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>257</v>
       </c>
@@ -12412,7 +12317,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:8">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>271</v>
       </c>
@@ -12438,7 +12343,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:8">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>271</v>
       </c>
@@ -12464,7 +12369,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:8">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>271</v>
       </c>
@@ -12490,7 +12395,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:8">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>271</v>
       </c>
@@ -12516,7 +12421,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:8">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>280</v>
       </c>
@@ -12542,7 +12447,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:8">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>280</v>
       </c>
@@ -12568,7 +12473,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:8">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>280</v>
       </c>
@@ -12594,7 +12499,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:8">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>280</v>
       </c>
@@ -12620,7 +12525,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:8">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>280</v>
       </c>
@@ -12646,7 +12551,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:8">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>286</v>
       </c>
@@ -12672,7 +12577,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:8">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>286</v>
       </c>
@@ -12698,7 +12603,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:8">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>286</v>
       </c>
@@ -12724,7 +12629,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:8">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>286</v>
       </c>
@@ -12750,7 +12655,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:8">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>291</v>
       </c>
@@ -12776,7 +12681,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:8">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>291</v>
       </c>
@@ -12802,7 +12707,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:8">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>291</v>
       </c>
@@ -12828,7 +12733,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:8">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>299</v>
       </c>
@@ -12854,7 +12759,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:8">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>299</v>
       </c>
@@ -12880,7 +12785,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:8">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>299</v>
       </c>
@@ -12906,7 +12811,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:8">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>304</v>
       </c>
@@ -12932,7 +12837,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:8">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>304</v>
       </c>
@@ -12958,7 +12863,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:8">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>304</v>
       </c>
@@ -12984,7 +12889,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:8">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>309</v>
       </c>
@@ -13010,7 +12915,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:8">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>309</v>
       </c>
@@ -13036,7 +12941,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:8">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>309</v>
       </c>
@@ -13062,7 +12967,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:8">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>309</v>
       </c>
@@ -13088,7 +12993,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:8">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>318</v>
       </c>
@@ -13114,7 +13019,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:8">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>318</v>
       </c>
@@ -13140,7 +13045,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:8">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>318</v>
       </c>
@@ -13166,7 +13071,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:8">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>318</v>
       </c>
@@ -13192,7 +13097,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:8">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>328</v>
       </c>
@@ -13218,7 +13123,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:8">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>346</v>
       </c>
@@ -13244,7 +13149,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:8">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>352</v>
       </c>
@@ -13270,7 +13175,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:8">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>358</v>
       </c>
@@ -13296,7 +13201,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:8">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>364</v>
       </c>
@@ -13322,7 +13227,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:8">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>370</v>
       </c>
@@ -13348,15 +13253,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:8">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>376</v>
       </c>
-      <c r="B83" s="1" t="s">
-        <v>381</v>
+      <c r="B83" s="1">
+        <v>23301</v>
       </c>
       <c r="C83" s="1">
-        <v>86400000</v>
+        <v>28800000</v>
       </c>
       <c r="D83" s="1">
         <v>1</v>
@@ -13388,9 +13293,9 @@
       <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -13416,7 +13321,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>96</v>
       </c>
@@ -13442,7 +13347,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>107</v>
       </c>
@@ -13468,7 +13373,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>115</v>
       </c>
@@ -13494,7 +13399,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>123</v>
       </c>
@@ -13520,7 +13425,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>128</v>
       </c>
@@ -13546,7 +13451,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>138</v>
       </c>
@@ -13572,7 +13477,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>144</v>
       </c>
@@ -13598,7 +13503,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>149</v>
       </c>
@@ -13624,7 +13529,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>158</v>
       </c>
@@ -13650,7 +13555,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>163</v>
       </c>
@@ -13676,7 +13581,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>168</v>
       </c>
@@ -13702,7 +13607,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>169</v>
       </c>
@@ -13728,7 +13633,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>187</v>
       </c>
@@ -13754,7 +13659,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>204</v>
       </c>
@@ -13780,7 +13685,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>221</v>
       </c>
@@ -13806,7 +13711,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>239</v>
       </c>
@@ -13832,7 +13737,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>257</v>
       </c>
@@ -13858,7 +13763,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>271</v>
       </c>
@@ -13884,7 +13789,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>280</v>
       </c>
@@ -13910,7 +13815,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>286</v>
       </c>
@@ -13936,7 +13841,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>291</v>
       </c>
@@ -13962,7 +13867,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>299</v>
       </c>
@@ -13988,7 +13893,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>304</v>
       </c>
@@ -14014,7 +13919,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>309</v>
       </c>
@@ -14040,7 +13945,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>318</v>
       </c>
@@ -14066,7 +13971,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>328</v>
       </c>
@@ -14092,7 +13997,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>346</v>
       </c>
@@ -14118,7 +14023,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>352</v>
       </c>
@@ -14144,7 +14049,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>358</v>
       </c>
@@ -14170,7 +14075,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>364</v>
       </c>
@@ -14196,7 +14101,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>370</v>
       </c>
@@ -14222,9 +14127,9 @@
         <v>100</v>
       </c>
     </row>
-    <row r="33" spans="1:8">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="B33" s="1">
         <v>315</v>
@@ -14248,9 +14153,9 @@
         <v>160</v>
       </c>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
       <c r="B34" s="1">
         <v>136</v>
@@ -14274,9 +14179,9 @@
         <v>160</v>
       </c>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
       <c r="B35" s="1">
         <v>35</v>
@@ -14300,9 +14205,9 @@
         <v>160</v>
       </c>
     </row>
-    <row r="36" spans="1:8">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="B36" s="1">
         <v>209</v>
@@ -14326,9 +14231,9 @@
         <v>200</v>
       </c>
     </row>
-    <row r="37" spans="1:8">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="B37" s="1">
         <v>0</v>
@@ -14352,9 +14257,9 @@
         <v>40</v>
       </c>
     </row>
-    <row r="38" spans="1:8">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
       <c r="B38" s="1">
         <v>0</v>
@@ -14378,9 +14283,9 @@
         <v>40</v>
       </c>
     </row>
-    <row r="39" spans="1:8">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="B39" s="1">
         <v>144</v>
@@ -14404,9 +14309,9 @@
         <v>160</v>
       </c>
     </row>
-    <row r="40" spans="1:8">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
       <c r="B40" s="1">
         <v>146</v>
@@ -14430,9 +14335,9 @@
         <v>160</v>
       </c>
     </row>
-    <row r="41" spans="1:8">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
       <c r="B41" s="1">
         <v>146</v>
@@ -14456,9 +14361,9 @@
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:8">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="B42" s="1">
         <v>146</v>
@@ -14482,9 +14387,9 @@
         <v>40</v>
       </c>
     </row>
-    <row r="43" spans="1:8">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="B43" s="1">
         <v>0</v>
@@ -14508,9 +14413,9 @@
         <v>40</v>
       </c>
     </row>
-    <row r="44" spans="1:8">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="B44" s="1">
         <v>0</v>
@@ -14534,9 +14439,9 @@
         <v>40</v>
       </c>
     </row>
-    <row r="45" spans="1:8">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
       <c r="B45" s="1">
         <v>0</v>
@@ -14560,9 +14465,9 @@
         <v>40</v>
       </c>
     </row>
-    <row r="46" spans="1:8">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="B46" s="1">
         <v>0</v>
@@ -14586,9 +14491,9 @@
         <v>40</v>
       </c>
     </row>
-    <row r="47" spans="1:8">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="B47" s="1">
         <v>0</v>
@@ -14612,9 +14517,9 @@
         <v>40</v>
       </c>
     </row>
-    <row r="48" spans="1:8">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="B48" s="1">
         <v>0</v>
@@ -14638,9 +14543,9 @@
         <v>40</v>
       </c>
     </row>
-    <row r="49" spans="1:8">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="B49" s="1">
         <v>0</v>
@@ -14664,9 +14569,9 @@
         <v>100</v>
       </c>
     </row>
-    <row r="50" spans="1:8">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="B50" s="1">
         <v>0</v>
@@ -14690,9 +14595,9 @@
         <v>100</v>
       </c>
     </row>
-    <row r="51" spans="1:8">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="B51" s="1">
         <v>0</v>
@@ -14716,9 +14621,9 @@
         <v>40</v>
       </c>
     </row>
-    <row r="52" spans="1:8">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
       <c r="B52" s="1">
         <v>0</v>
@@ -14742,7 +14647,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="53" spans="1:8">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>376</v>
       </c>
@@ -14780,17 +14685,17 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>5</v>
@@ -14805,30 +14710,30 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>399</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>400</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>403</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>404</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>405</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>406</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>407</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>408</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -14848,10 +14753,10 @@
         <v>8</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>51</v>
       </c>
@@ -14871,10 +14776,10 @@
         <v>8</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>101</v>
       </c>
@@ -14894,10 +14799,10 @@
         <v>8</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>427</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>151</v>
       </c>
@@ -14917,10 +14822,10 @@
         <v>8</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>201</v>
       </c>
@@ -14940,10 +14845,10 @@
         <v>8</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>251</v>
       </c>
@@ -14963,10 +14868,10 @@
         <v>8</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>46</v>
       </c>
@@ -14986,7 +14891,7 @@
         <v>8</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add acc sette buffer
</commit_message>
<xml_diff>
--- a/gu_in/Map.edf/Sette.xlsx
+++ b/gu_in/Map.edf/Sette.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project RF X\Parser_Public_Releases\Parser_1.0.2\database\gu_in\Map.edf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7E20926-11D6-43F5-B4ED-F7103AAD6880}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4D114AE-8349-4A21-9797-693A6A3D691C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -836,7 +836,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="936" uniqueCount="428">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="937" uniqueCount="430">
   <si>
     <t>char[32]</t>
   </si>
@@ -2120,6 +2120,12 @@
   </si>
   <si>
     <t>Windy Cave</t>
+  </si>
+  <si>
+    <t>sd131A8</t>
+  </si>
+  <si>
+    <t>bd131A8</t>
   </si>
 </sst>
 </file>
@@ -4176,7 +4182,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:J233"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A206" workbookViewId="0">
+    <sheetView topLeftCell="A206" workbookViewId="0">
       <selection activeCell="P231" sqref="P231"/>
     </sheetView>
   </sheetViews>
@@ -13287,10 +13293,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:H53"/>
+  <dimension ref="A1:H54"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="P45" sqref="P45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14649,28 +14655,54 @@
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>376</v>
+        <v>428</v>
       </c>
       <c r="B53" s="1">
         <v>0</v>
       </c>
       <c r="C53" s="1">
-        <v>-2581</v>
+        <v>3388</v>
       </c>
       <c r="D53" s="1">
-        <v>-75</v>
+        <v>-111</v>
       </c>
       <c r="E53" s="1">
-        <v>2486</v>
+        <v>-3561</v>
       </c>
       <c r="F53" s="1">
-        <v>200</v>
+        <v>40</v>
       </c>
       <c r="G53" s="1">
-        <v>200</v>
+        <v>28</v>
       </c>
       <c r="H53" s="1">
-        <v>200</v>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>429</v>
+      </c>
+      <c r="B54" s="1">
+        <v>0</v>
+      </c>
+      <c r="C54" s="1">
+        <v>3388</v>
+      </c>
+      <c r="D54" s="1">
+        <v>-111</v>
+      </c>
+      <c r="E54" s="1">
+        <v>-3561</v>
+      </c>
+      <c r="F54" s="1">
+        <v>40</v>
+      </c>
+      <c r="G54" s="1">
+        <v>28</v>
+      </c>
+      <c r="H54" s="1">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
buffer sette cora bells
</commit_message>
<xml_diff>
--- a/gu_in/Map.edf/Sette.xlsx
+++ b/gu_in/Map.edf/Sette.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project RF X\Parser_Public_Releases\Parser_1.0.2\database\gu_in\Map.edf\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\emay.dev\Parser_1.0.2\Database\gu_in\Map.edf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4D114AE-8349-4A21-9797-693A6A3D691C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6790F68C-605A-4533-A666-2F90D5328400}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5235" yWindow="1320" windowWidth="18480" windowHeight="11205" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -31,8 +31,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -836,7 +834,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="937" uniqueCount="430">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="941" uniqueCount="434">
   <si>
     <t>char[32]</t>
   </si>
@@ -2126,13 +2124,25 @@
   </si>
   <si>
     <t>bd131A8</t>
+  </si>
+  <si>
+    <t>sd131A9</t>
+  </si>
+  <si>
+    <t>bd131A9</t>
+  </si>
+  <si>
+    <t>sd131B0</t>
+  </si>
+  <si>
+    <t>bd131B0</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -2204,9 +2214,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2244,7 +2254,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2350,7 +2360,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2492,7 +2502,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2506,13 +2516,13 @@
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="19.140625" customWidth="1"/>
     <col min="3" max="3" width="30" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2523,7 +2533,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -2534,7 +2544,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -2545,7 +2555,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -2556,7 +2566,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -2567,7 +2577,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -2578,7 +2588,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -2589,7 +2599,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -2600,7 +2610,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3">
       <c r="A9" s="1" t="s">
         <v>5</v>
       </c>
@@ -2611,7 +2621,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3">
       <c r="A10" s="1" t="s">
         <v>5</v>
       </c>
@@ -2622,7 +2632,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3">
       <c r="A11" s="1" t="s">
         <v>4</v>
       </c>
@@ -2633,7 +2643,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3">
       <c r="A12" s="1" t="s">
         <v>5</v>
       </c>
@@ -2644,7 +2654,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3">
       <c r="A13" s="1" t="s">
         <v>5</v>
       </c>
@@ -2655,7 +2665,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3">
       <c r="A14" s="1" t="s">
         <v>5</v>
       </c>
@@ -2666,7 +2676,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3">
       <c r="A15" s="1" t="s">
         <v>5</v>
       </c>
@@ -2677,7 +2687,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3">
       <c r="A16" s="1" t="s">
         <v>6</v>
       </c>
@@ -2688,7 +2698,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3">
       <c r="A17" s="1" t="s">
         <v>6</v>
       </c>
@@ -2699,7 +2709,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3">
       <c r="A18" s="1" t="s">
         <v>5</v>
       </c>
@@ -2710,7 +2720,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3">
       <c r="A19" s="1" t="s">
         <v>5</v>
       </c>
@@ -2721,7 +2731,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3">
       <c r="A20" s="1" t="s">
         <v>6</v>
       </c>
@@ -2732,7 +2742,7 @@
         <v>7475</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3">
       <c r="A21" s="1" t="s">
         <v>6</v>
       </c>
@@ -2743,7 +2753,7 @@
         <v>7474</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3">
       <c r="A22" s="1" t="s">
         <v>6</v>
       </c>
@@ -2754,7 +2764,7 @@
         <v>100782</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3">
       <c r="A23" s="1" t="s">
         <v>6</v>
       </c>
@@ -2765,7 +2775,7 @@
         <v>108015</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3">
       <c r="A24" s="1" t="s">
         <v>6</v>
       </c>
@@ -2790,7 +2800,7 @@
       <selection activeCell="W18" sqref="W18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="25.7109375" customWidth="1"/>
     <col min="2" max="2" width="27.7109375" customWidth="1"/>
@@ -2806,7 +2816,7 @@
     <col min="22" max="22" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2892,7 +2902,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28">
       <c r="A2" s="1" t="s">
         <v>37</v>
       </c>
@@ -2978,7 +2988,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28">
       <c r="A3" s="1" t="s">
         <v>65</v>
       </c>
@@ -3064,7 +3074,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:28">
       <c r="A4" s="1" t="s">
         <v>69</v>
       </c>
@@ -3150,7 +3160,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28">
       <c r="A5" s="1" t="s">
         <v>71</v>
       </c>
@@ -3236,7 +3246,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:28">
       <c r="A6" s="1" t="s">
         <v>73</v>
       </c>
@@ -3322,7 +3332,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:28">
       <c r="A7" s="1" t="s">
         <v>76</v>
       </c>
@@ -3408,7 +3418,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:28">
       <c r="A8" s="1" t="s">
         <v>80</v>
       </c>
@@ -3494,7 +3504,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:28">
       <c r="A9" s="1" t="s">
         <v>68</v>
       </c>
@@ -3580,7 +3590,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:28">
       <c r="A10" s="1" t="s">
         <v>68</v>
       </c>
@@ -3666,7 +3676,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:28">
       <c r="A11" s="1" t="s">
         <v>68</v>
       </c>
@@ -3752,7 +3762,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:28">
       <c r="A12" s="1" t="s">
         <v>68</v>
       </c>
@@ -3838,7 +3848,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:28">
       <c r="A13" s="1" t="s">
         <v>68</v>
       </c>
@@ -3936,9 +3946,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -3964,7 +3974,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8">
       <c r="A2" s="1" t="s">
         <v>40</v>
       </c>
@@ -4001,9 +4011,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -4020,7 +4030,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" s="1" t="s">
         <v>89</v>
       </c>
@@ -4037,7 +4047,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" s="1">
         <v>51</v>
       </c>
@@ -4054,7 +4064,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4" s="1">
         <v>288</v>
       </c>
@@ -4071,7 +4081,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5" s="1">
         <v>72</v>
       </c>
@@ -4088,7 +4098,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6" s="1">
         <v>289</v>
       </c>
@@ -4105,7 +4115,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7" s="1">
         <v>112</v>
       </c>
@@ -4122,7 +4132,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="A8" s="1">
         <v>134</v>
       </c>
@@ -4139,7 +4149,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9" s="1">
         <v>280</v>
       </c>
@@ -4156,7 +4166,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5">
       <c r="A10" s="1">
         <v>232</v>
       </c>
@@ -4186,13 +4196,13 @@
       <selection activeCell="P231" sqref="P231"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="19.140625" customWidth="1"/>
     <col min="2" max="2" width="21.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -4224,7 +4234,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10">
       <c r="A2" s="1" t="s">
         <v>96</v>
       </c>
@@ -4256,7 +4266,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10">
       <c r="A3" s="1" t="s">
         <v>107</v>
       </c>
@@ -4270,7 +4280,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10">
       <c r="A4" s="1" t="s">
         <v>107</v>
       </c>
@@ -4302,7 +4312,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10">
       <c r="A5" s="1" t="s">
         <v>107</v>
       </c>
@@ -4334,7 +4344,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10">
       <c r="A6" s="1" t="s">
         <v>107</v>
       </c>
@@ -4366,7 +4376,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10">
       <c r="A7" s="1" t="s">
         <v>107</v>
       </c>
@@ -4398,7 +4408,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10">
       <c r="A8" s="1" t="s">
         <v>115</v>
       </c>
@@ -4412,7 +4422,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10">
       <c r="A9" s="1" t="s">
         <v>115</v>
       </c>
@@ -4444,7 +4454,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10">
       <c r="A10" s="1" t="s">
         <v>115</v>
       </c>
@@ -4476,7 +4486,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10">
       <c r="A11" s="1" t="s">
         <v>115</v>
       </c>
@@ -4508,7 +4518,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10">
       <c r="A12" s="1" t="s">
         <v>115</v>
       </c>
@@ -4540,7 +4550,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10">
       <c r="A13" s="1" t="s">
         <v>123</v>
       </c>
@@ -4554,7 +4564,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10">
       <c r="A14" s="1" t="s">
         <v>123</v>
       </c>
@@ -4586,7 +4596,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10">
       <c r="A15" s="1" t="s">
         <v>123</v>
       </c>
@@ -4618,7 +4628,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10">
       <c r="A16" s="1" t="s">
         <v>123</v>
       </c>
@@ -4650,7 +4660,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10">
       <c r="A17" s="1" t="s">
         <v>123</v>
       </c>
@@ -4682,7 +4692,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10">
       <c r="A18" s="1" t="s">
         <v>128</v>
       </c>
@@ -4696,7 +4706,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10">
       <c r="A19" s="1" t="s">
         <v>128</v>
       </c>
@@ -4728,7 +4738,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10">
       <c r="A20" s="1" t="s">
         <v>128</v>
       </c>
@@ -4760,7 +4770,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10">
       <c r="A21" s="1" t="s">
         <v>128</v>
       </c>
@@ -4792,7 +4802,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10">
       <c r="A22" s="1" t="s">
         <v>128</v>
       </c>
@@ -4824,7 +4834,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10">
       <c r="A23" s="1" t="s">
         <v>138</v>
       </c>
@@ -4838,7 +4848,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10">
       <c r="A24" s="1" t="s">
         <v>138</v>
       </c>
@@ -4870,7 +4880,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10">
       <c r="A25" s="1" t="s">
         <v>138</v>
       </c>
@@ -4902,7 +4912,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10">
       <c r="A26" s="1" t="s">
         <v>138</v>
       </c>
@@ -4934,7 +4944,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10">
       <c r="A27" s="1" t="s">
         <v>138</v>
       </c>
@@ -4966,7 +4976,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10">
       <c r="A28" s="1" t="s">
         <v>144</v>
       </c>
@@ -4980,7 +4990,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10">
       <c r="A29" s="1" t="s">
         <v>144</v>
       </c>
@@ -5012,7 +5022,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10">
       <c r="A30" s="1" t="s">
         <v>144</v>
       </c>
@@ -5044,7 +5054,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10">
       <c r="A31" s="1" t="s">
         <v>144</v>
       </c>
@@ -5076,7 +5086,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10">
       <c r="A32" s="1" t="s">
         <v>144</v>
       </c>
@@ -5108,7 +5118,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10">
       <c r="A33" s="1" t="s">
         <v>149</v>
       </c>
@@ -5122,7 +5132,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10">
       <c r="A34" s="1" t="s">
         <v>149</v>
       </c>
@@ -5154,7 +5164,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10">
       <c r="A35" s="1" t="s">
         <v>149</v>
       </c>
@@ -5186,7 +5196,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10">
       <c r="A36" s="1" t="s">
         <v>149</v>
       </c>
@@ -5218,7 +5228,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10">
       <c r="A37" s="1" t="s">
         <v>149</v>
       </c>
@@ -5250,7 +5260,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10">
       <c r="A38" s="1" t="s">
         <v>158</v>
       </c>
@@ -5264,7 +5274,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10">
       <c r="A39" s="1" t="s">
         <v>158</v>
       </c>
@@ -5296,7 +5306,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10">
       <c r="A40" s="1" t="s">
         <v>158</v>
       </c>
@@ -5328,7 +5338,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10">
       <c r="A41" s="1" t="s">
         <v>158</v>
       </c>
@@ -5360,7 +5370,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10">
       <c r="A42" s="1" t="s">
         <v>158</v>
       </c>
@@ -5392,7 +5402,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10">
       <c r="A43" s="1" t="s">
         <v>163</v>
       </c>
@@ -5406,7 +5416,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10">
       <c r="A44" s="1" t="s">
         <v>163</v>
       </c>
@@ -5438,7 +5448,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10">
       <c r="A45" s="1" t="s">
         <v>163</v>
       </c>
@@ -5470,7 +5480,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10">
       <c r="A46" s="1" t="s">
         <v>163</v>
       </c>
@@ -5502,7 +5512,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10">
       <c r="A47" s="1" t="s">
         <v>163</v>
       </c>
@@ -5534,7 +5544,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10">
       <c r="A48" s="1" t="s">
         <v>169</v>
       </c>
@@ -5548,7 +5558,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10">
       <c r="A49" s="1" t="s">
         <v>169</v>
       </c>
@@ -5580,7 +5590,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10">
       <c r="A50" s="1" t="s">
         <v>169</v>
       </c>
@@ -5612,7 +5622,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10">
       <c r="A51" s="1" t="s">
         <v>169</v>
       </c>
@@ -5644,7 +5654,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10">
       <c r="A52" s="1" t="s">
         <v>169</v>
       </c>
@@ -5676,7 +5686,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10">
       <c r="A53" s="1" t="s">
         <v>169</v>
       </c>
@@ -5708,7 +5718,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10">
       <c r="A54" s="1" t="s">
         <v>169</v>
       </c>
@@ -5740,7 +5750,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10">
       <c r="A55" s="1" t="s">
         <v>169</v>
       </c>
@@ -5772,7 +5782,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10">
       <c r="A56" s="1" t="s">
         <v>169</v>
       </c>
@@ -5804,7 +5814,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10">
       <c r="A57" s="1" t="s">
         <v>169</v>
       </c>
@@ -5836,7 +5846,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10">
       <c r="A58" s="1" t="s">
         <v>169</v>
       </c>
@@ -5868,7 +5878,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10">
       <c r="A59" s="1" t="s">
         <v>169</v>
       </c>
@@ -5900,7 +5910,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10">
       <c r="A60" s="1" t="s">
         <v>169</v>
       </c>
@@ -5932,7 +5942,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10">
       <c r="A61" s="1" t="s">
         <v>169</v>
       </c>
@@ -5964,7 +5974,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10">
       <c r="A62" s="1" t="s">
         <v>169</v>
       </c>
@@ -5996,7 +6006,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10">
       <c r="A63" s="1" t="s">
         <v>169</v>
       </c>
@@ -6028,7 +6038,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10">
       <c r="A64" s="1" t="s">
         <v>169</v>
       </c>
@@ -6060,7 +6070,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10">
       <c r="A65" s="1" t="s">
         <v>187</v>
       </c>
@@ -6074,7 +6084,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10">
       <c r="A66" s="1" t="s">
         <v>187</v>
       </c>
@@ -6106,7 +6116,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10">
       <c r="A67" s="1" t="s">
         <v>187</v>
       </c>
@@ -6138,7 +6148,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10">
       <c r="A68" s="1" t="s">
         <v>187</v>
       </c>
@@ -6170,7 +6180,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10">
       <c r="A69" s="1" t="s">
         <v>187</v>
       </c>
@@ -6202,7 +6212,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10">
       <c r="A70" s="1" t="s">
         <v>187</v>
       </c>
@@ -6234,7 +6244,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10">
       <c r="A71" s="1" t="s">
         <v>187</v>
       </c>
@@ -6266,7 +6276,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10">
       <c r="A72" s="1" t="s">
         <v>187</v>
       </c>
@@ -6298,7 +6308,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10">
       <c r="A73" s="1" t="s">
         <v>187</v>
       </c>
@@ -6330,7 +6340,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10">
       <c r="A74" s="1" t="s">
         <v>187</v>
       </c>
@@ -6362,7 +6372,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10">
       <c r="A75" s="1" t="s">
         <v>187</v>
       </c>
@@ -6394,7 +6404,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10">
       <c r="A76" s="1" t="s">
         <v>187</v>
       </c>
@@ -6426,7 +6436,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10">
       <c r="A77" s="1" t="s">
         <v>187</v>
       </c>
@@ -6458,7 +6468,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:10">
       <c r="A78" s="1" t="s">
         <v>187</v>
       </c>
@@ -6490,7 +6500,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:10">
       <c r="A79" s="1" t="s">
         <v>187</v>
       </c>
@@ -6522,7 +6532,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:10">
       <c r="A80" s="1" t="s">
         <v>187</v>
       </c>
@@ -6554,7 +6564,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:10">
       <c r="A81" s="1" t="s">
         <v>187</v>
       </c>
@@ -6586,7 +6596,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:10">
       <c r="A82" s="1" t="s">
         <v>204</v>
       </c>
@@ -6600,7 +6610,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:10">
       <c r="A83" s="1" t="s">
         <v>204</v>
       </c>
@@ -6632,7 +6642,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:10">
       <c r="A84" s="1" t="s">
         <v>204</v>
       </c>
@@ -6664,7 +6674,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:10">
       <c r="A85" s="1" t="s">
         <v>204</v>
       </c>
@@ -6696,7 +6706,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:10">
       <c r="A86" s="1" t="s">
         <v>204</v>
       </c>
@@ -6728,7 +6738,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:10">
       <c r="A87" s="1" t="s">
         <v>204</v>
       </c>
@@ -6760,7 +6770,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:10">
       <c r="A88" s="1" t="s">
         <v>204</v>
       </c>
@@ -6792,7 +6802,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:10">
       <c r="A89" s="1" t="s">
         <v>204</v>
       </c>
@@ -6824,7 +6834,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:10">
       <c r="A90" s="1" t="s">
         <v>204</v>
       </c>
@@ -6856,7 +6866,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:10">
       <c r="A91" s="1" t="s">
         <v>204</v>
       </c>
@@ -6888,7 +6898,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:10">
       <c r="A92" s="1" t="s">
         <v>204</v>
       </c>
@@ -6920,7 +6930,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:10">
       <c r="A93" s="1" t="s">
         <v>204</v>
       </c>
@@ -6952,7 +6962,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:10">
       <c r="A94" s="1" t="s">
         <v>204</v>
       </c>
@@ -6984,7 +6994,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:10">
       <c r="A95" s="1" t="s">
         <v>204</v>
       </c>
@@ -7016,7 +7026,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:10">
       <c r="A96" s="1" t="s">
         <v>204</v>
       </c>
@@ -7048,7 +7058,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:10">
       <c r="A97" s="1" t="s">
         <v>204</v>
       </c>
@@ -7080,7 +7090,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:10">
       <c r="A98" s="1" t="s">
         <v>204</v>
       </c>
@@ -7112,7 +7122,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:10">
       <c r="A99" s="1" t="s">
         <v>221</v>
       </c>
@@ -7126,7 +7136,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:10">
       <c r="A100" s="1" t="s">
         <v>221</v>
       </c>
@@ -7158,7 +7168,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:10">
       <c r="A101" s="1" t="s">
         <v>221</v>
       </c>
@@ -7190,7 +7200,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:10">
       <c r="A102" s="1" t="s">
         <v>221</v>
       </c>
@@ -7222,7 +7232,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:10">
       <c r="A103" s="1" t="s">
         <v>221</v>
       </c>
@@ -7254,7 +7264,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:10">
       <c r="A104" s="1" t="s">
         <v>221</v>
       </c>
@@ -7286,7 +7296,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:10">
       <c r="A105" s="1" t="s">
         <v>221</v>
       </c>
@@ -7318,7 +7328,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:10">
       <c r="A106" s="1" t="s">
         <v>221</v>
       </c>
@@ -7350,7 +7360,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:10">
       <c r="A107" s="1" t="s">
         <v>221</v>
       </c>
@@ -7382,7 +7392,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:10">
       <c r="A108" s="1" t="s">
         <v>221</v>
       </c>
@@ -7414,7 +7424,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:10">
       <c r="A109" s="1" t="s">
         <v>221</v>
       </c>
@@ -7446,7 +7456,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:10">
       <c r="A110" s="1" t="s">
         <v>221</v>
       </c>
@@ -7478,7 +7488,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:10">
       <c r="A111" s="1" t="s">
         <v>221</v>
       </c>
@@ -7510,7 +7520,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:10">
       <c r="A112" s="1" t="s">
         <v>221</v>
       </c>
@@ -7542,7 +7552,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:10">
       <c r="A113" s="1" t="s">
         <v>221</v>
       </c>
@@ -7574,7 +7584,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:10">
       <c r="A114" s="1" t="s">
         <v>221</v>
       </c>
@@ -7606,7 +7616,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:10">
       <c r="A115" s="1" t="s">
         <v>221</v>
       </c>
@@ -7638,7 +7648,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:10">
       <c r="A116" s="1" t="s">
         <v>239</v>
       </c>
@@ -7652,7 +7662,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:10">
       <c r="A117" s="1" t="s">
         <v>239</v>
       </c>
@@ -7684,7 +7694,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:10">
       <c r="A118" s="1" t="s">
         <v>239</v>
       </c>
@@ -7716,7 +7726,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:10">
       <c r="A119" s="1" t="s">
         <v>239</v>
       </c>
@@ -7748,7 +7758,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:10">
       <c r="A120" s="1" t="s">
         <v>239</v>
       </c>
@@ -7780,7 +7790,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:10">
       <c r="A121" s="1" t="s">
         <v>239</v>
       </c>
@@ -7812,7 +7822,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:10">
       <c r="A122" s="1" t="s">
         <v>239</v>
       </c>
@@ -7844,7 +7854,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:10">
       <c r="A123" s="1" t="s">
         <v>239</v>
       </c>
@@ -7876,7 +7886,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:10">
       <c r="A124" s="1" t="s">
         <v>239</v>
       </c>
@@ -7908,7 +7918,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:10">
       <c r="A125" s="1" t="s">
         <v>239</v>
       </c>
@@ -7940,7 +7950,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:10">
       <c r="A126" s="1" t="s">
         <v>239</v>
       </c>
@@ -7972,7 +7982,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:10">
       <c r="A127" s="1" t="s">
         <v>239</v>
       </c>
@@ -8004,7 +8014,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:10">
       <c r="A128" s="1" t="s">
         <v>239</v>
       </c>
@@ -8036,7 +8046,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="129" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:10">
       <c r="A129" s="1" t="s">
         <v>239</v>
       </c>
@@ -8068,7 +8078,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="130" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:10">
       <c r="A130" s="1" t="s">
         <v>239</v>
       </c>
@@ -8100,7 +8110,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="131" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:10">
       <c r="A131" s="1" t="s">
         <v>239</v>
       </c>
@@ -8132,7 +8142,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="132" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:10">
       <c r="A132" s="1" t="s">
         <v>239</v>
       </c>
@@ -8164,7 +8174,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="133" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:10">
       <c r="A133" s="1" t="s">
         <v>257</v>
       </c>
@@ -8178,7 +8188,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:10">
       <c r="A134" s="1" t="s">
         <v>257</v>
       </c>
@@ -8210,7 +8220,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="135" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:10">
       <c r="A135" s="1" t="s">
         <v>257</v>
       </c>
@@ -8242,7 +8252,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="136" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:10">
       <c r="A136" s="1" t="s">
         <v>257</v>
       </c>
@@ -8274,7 +8284,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="137" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:10">
       <c r="A137" s="1" t="s">
         <v>257</v>
       </c>
@@ -8306,7 +8316,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="138" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:10">
       <c r="A138" s="1" t="s">
         <v>257</v>
       </c>
@@ -8338,7 +8348,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="139" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:10">
       <c r="A139" s="1" t="s">
         <v>257</v>
       </c>
@@ -8370,7 +8380,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="140" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:10">
       <c r="A140" s="1" t="s">
         <v>257</v>
       </c>
@@ -8402,7 +8412,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="141" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:10">
       <c r="A141" s="1" t="s">
         <v>257</v>
       </c>
@@ -8434,7 +8444,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="142" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:10">
       <c r="A142" s="1" t="s">
         <v>257</v>
       </c>
@@ -8466,7 +8476,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="143" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:10">
       <c r="A143" s="1" t="s">
         <v>257</v>
       </c>
@@ -8498,7 +8508,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="144" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:10">
       <c r="A144" s="1" t="s">
         <v>257</v>
       </c>
@@ -8530,7 +8540,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="145" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:10">
       <c r="A145" s="1" t="s">
         <v>257</v>
       </c>
@@ -8562,7 +8572,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="146" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:10">
       <c r="A146" s="1" t="s">
         <v>271</v>
       </c>
@@ -8576,7 +8586,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:10">
       <c r="A147" s="1" t="s">
         <v>271</v>
       </c>
@@ -8608,7 +8618,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="148" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:10">
       <c r="A148" s="1" t="s">
         <v>271</v>
       </c>
@@ -8640,7 +8650,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="149" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:10">
       <c r="A149" s="1" t="s">
         <v>271</v>
       </c>
@@ -8672,7 +8682,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="150" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:10">
       <c r="A150" s="1" t="s">
         <v>271</v>
       </c>
@@ -8704,7 +8714,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="151" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:10">
       <c r="A151" s="1" t="s">
         <v>280</v>
       </c>
@@ -8718,7 +8728,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:10">
       <c r="A152" s="1" t="s">
         <v>280</v>
       </c>
@@ -8750,7 +8760,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="153" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:10">
       <c r="A153" s="1" t="s">
         <v>280</v>
       </c>
@@ -8782,7 +8792,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="154" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:10">
       <c r="A154" s="1" t="s">
         <v>280</v>
       </c>
@@ -8814,7 +8824,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="155" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:10">
       <c r="A155" s="1" t="s">
         <v>280</v>
       </c>
@@ -8846,7 +8856,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="156" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:10">
       <c r="A156" s="1" t="s">
         <v>286</v>
       </c>
@@ -8860,7 +8870,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:10">
       <c r="A157" s="1" t="s">
         <v>286</v>
       </c>
@@ -8892,7 +8902,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="158" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:10">
       <c r="A158" s="1" t="s">
         <v>286</v>
       </c>
@@ -8924,7 +8934,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="159" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:10">
       <c r="A159" s="1" t="s">
         <v>286</v>
       </c>
@@ -8956,7 +8966,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="160" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:10">
       <c r="A160" s="1" t="s">
         <v>286</v>
       </c>
@@ -8988,7 +8998,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="161" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:10">
       <c r="A161" s="1" t="s">
         <v>291</v>
       </c>
@@ -9002,7 +9012,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="162" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:10">
       <c r="A162" s="1" t="s">
         <v>291</v>
       </c>
@@ -9034,7 +9044,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="163" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:10">
       <c r="A163" s="1" t="s">
         <v>291</v>
       </c>
@@ -9066,7 +9076,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="164" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:10">
       <c r="A164" s="1" t="s">
         <v>291</v>
       </c>
@@ -9098,7 +9108,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="165" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:10">
       <c r="A165" s="1" t="s">
         <v>291</v>
       </c>
@@ -9130,7 +9140,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="166" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:10">
       <c r="A166" s="1" t="s">
         <v>299</v>
       </c>
@@ -9144,7 +9154,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="167" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:10">
       <c r="A167" s="1" t="s">
         <v>299</v>
       </c>
@@ -9176,7 +9186,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="168" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:10">
       <c r="A168" s="1" t="s">
         <v>299</v>
       </c>
@@ -9208,7 +9218,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="169" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:10">
       <c r="A169" s="1" t="s">
         <v>299</v>
       </c>
@@ -9240,7 +9250,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="170" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:10">
       <c r="A170" s="1" t="s">
         <v>299</v>
       </c>
@@ -9272,7 +9282,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="171" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:10">
       <c r="A171" s="1" t="s">
         <v>304</v>
       </c>
@@ -9286,7 +9296,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="172" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:10">
       <c r="A172" s="1" t="s">
         <v>304</v>
       </c>
@@ -9318,7 +9328,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="173" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:10">
       <c r="A173" s="1" t="s">
         <v>304</v>
       </c>
@@ -9350,7 +9360,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="174" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:10">
       <c r="A174" s="1" t="s">
         <v>304</v>
       </c>
@@ -9382,7 +9392,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="175" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:10">
       <c r="A175" s="1" t="s">
         <v>304</v>
       </c>
@@ -9414,7 +9424,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="176" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:10">
       <c r="A176" s="1" t="s">
         <v>309</v>
       </c>
@@ -9428,7 +9438,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="177" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:10">
       <c r="A177" s="1" t="s">
         <v>309</v>
       </c>
@@ -9460,7 +9470,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="178" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:10">
       <c r="A178" s="1" t="s">
         <v>309</v>
       </c>
@@ -9492,7 +9502,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="179" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:10">
       <c r="A179" s="1" t="s">
         <v>309</v>
       </c>
@@ -9524,7 +9534,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="180" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:10">
       <c r="A180" s="1" t="s">
         <v>309</v>
       </c>
@@ -9556,7 +9566,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="181" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:10">
       <c r="A181" s="1" t="s">
         <v>318</v>
       </c>
@@ -9570,7 +9580,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="182" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:10">
       <c r="A182" s="1" t="s">
         <v>318</v>
       </c>
@@ -9602,7 +9612,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="183" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:10">
       <c r="A183" s="1" t="s">
         <v>318</v>
       </c>
@@ -9634,7 +9644,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="184" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:10">
       <c r="A184" s="1" t="s">
         <v>318</v>
       </c>
@@ -9666,7 +9676,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="185" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:10">
       <c r="A185" s="1" t="s">
         <v>318</v>
       </c>
@@ -9698,7 +9708,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="186" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:10">
       <c r="A186" s="1" t="s">
         <v>318</v>
       </c>
@@ -9730,7 +9740,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="187" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:10">
       <c r="A187" s="1" t="s">
         <v>318</v>
       </c>
@@ -9762,7 +9772,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="188" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:10">
       <c r="A188" s="1" t="s">
         <v>318</v>
       </c>
@@ -9794,7 +9804,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="189" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:10">
       <c r="A189" s="1" t="s">
         <v>318</v>
       </c>
@@ -9826,7 +9836,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="190" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:10">
       <c r="A190" s="1" t="s">
         <v>328</v>
       </c>
@@ -9840,7 +9850,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="191" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:10">
       <c r="A191" s="1" t="s">
         <v>328</v>
       </c>
@@ -9872,7 +9882,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="192" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:10">
       <c r="A192" s="1" t="s">
         <v>328</v>
       </c>
@@ -9904,7 +9914,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="193" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:10">
       <c r="A193" s="1" t="s">
         <v>328</v>
       </c>
@@ -9936,7 +9946,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="194" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:10">
       <c r="A194" s="1" t="s">
         <v>328</v>
       </c>
@@ -9968,7 +9978,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="195" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:10">
       <c r="A195" s="1" t="s">
         <v>328</v>
       </c>
@@ -10000,7 +10010,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="196" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:10">
       <c r="A196" s="1" t="s">
         <v>328</v>
       </c>
@@ -10032,7 +10042,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="197" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:10">
       <c r="A197" s="1" t="s">
         <v>328</v>
       </c>
@@ -10064,7 +10074,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="198" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:10">
       <c r="A198" s="1" t="s">
         <v>328</v>
       </c>
@@ -10096,7 +10106,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="199" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:10">
       <c r="A199" s="1" t="s">
         <v>328</v>
       </c>
@@ -10128,7 +10138,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="200" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:10">
       <c r="A200" s="1" t="s">
         <v>328</v>
       </c>
@@ -10160,7 +10170,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="201" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:10">
       <c r="A201" s="1" t="s">
         <v>328</v>
       </c>
@@ -10192,7 +10202,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="202" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:10">
       <c r="A202" s="1" t="s">
         <v>328</v>
       </c>
@@ -10224,7 +10234,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="203" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:10">
       <c r="A203" s="1" t="s">
         <v>328</v>
       </c>
@@ -10256,7 +10266,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="204" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:10">
       <c r="A204" s="1" t="s">
         <v>328</v>
       </c>
@@ -10288,7 +10298,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="205" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:10">
       <c r="A205" s="1" t="s">
         <v>328</v>
       </c>
@@ -10320,7 +10330,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="206" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:10">
       <c r="A206" s="1" t="s">
         <v>328</v>
       </c>
@@ -10352,7 +10362,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="207" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:10">
       <c r="A207" s="1" t="s">
         <v>346</v>
       </c>
@@ -10366,7 +10376,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="208" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:10">
       <c r="A208" s="1" t="s">
         <v>346</v>
       </c>
@@ -10398,7 +10408,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="209" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:10">
       <c r="A209" s="1" t="s">
         <v>346</v>
       </c>
@@ -10430,7 +10440,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="210" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:10">
       <c r="A210" s="1" t="s">
         <v>346</v>
       </c>
@@ -10462,7 +10472,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="211" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:10">
       <c r="A211" s="1" t="s">
         <v>346</v>
       </c>
@@ -10494,7 +10504,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="212" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:10">
       <c r="A212" s="1" t="s">
         <v>352</v>
       </c>
@@ -10508,7 +10518,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="213" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:10">
       <c r="A213" s="1" t="s">
         <v>352</v>
       </c>
@@ -10540,7 +10550,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="214" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:10">
       <c r="A214" s="1" t="s">
         <v>352</v>
       </c>
@@ -10572,7 +10582,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="215" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:10">
       <c r="A215" s="1" t="s">
         <v>352</v>
       </c>
@@ -10604,7 +10614,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="216" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:10">
       <c r="A216" s="1" t="s">
         <v>352</v>
       </c>
@@ -10636,7 +10646,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="217" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:10">
       <c r="A217" s="1" t="s">
         <v>358</v>
       </c>
@@ -10650,7 +10660,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="218" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:10">
       <c r="A218" s="1" t="s">
         <v>358</v>
       </c>
@@ -10682,7 +10692,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="219" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:10">
       <c r="A219" s="1" t="s">
         <v>358</v>
       </c>
@@ -10714,7 +10724,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="220" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:10">
       <c r="A220" s="1" t="s">
         <v>358</v>
       </c>
@@ -10746,7 +10756,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="221" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:10">
       <c r="A221" s="1" t="s">
         <v>358</v>
       </c>
@@ -10778,7 +10788,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="222" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:10">
       <c r="A222" s="1" t="s">
         <v>364</v>
       </c>
@@ -10792,7 +10802,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="223" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:10">
       <c r="A223" s="1" t="s">
         <v>364</v>
       </c>
@@ -10824,7 +10834,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="224" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:10">
       <c r="A224" s="1" t="s">
         <v>364</v>
       </c>
@@ -10856,7 +10866,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="225" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:10">
       <c r="A225" s="1" t="s">
         <v>364</v>
       </c>
@@ -10888,7 +10898,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="226" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:10">
       <c r="A226" s="1" t="s">
         <v>364</v>
       </c>
@@ -10920,7 +10930,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="227" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:10">
       <c r="A227" s="1" t="s">
         <v>370</v>
       </c>
@@ -10934,7 +10944,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="228" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:10">
       <c r="A228" s="1" t="s">
         <v>370</v>
       </c>
@@ -10966,7 +10976,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="229" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:10">
       <c r="A229" s="1" t="s">
         <v>370</v>
       </c>
@@ -10998,7 +11008,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="230" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:10">
       <c r="A230" s="1" t="s">
         <v>370</v>
       </c>
@@ -11030,7 +11040,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="231" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:10">
       <c r="A231" s="1" t="s">
         <v>370</v>
       </c>
@@ -11062,7 +11072,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="232" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:10">
       <c r="A232" s="1" t="s">
         <v>376</v>
       </c>
@@ -11076,7 +11086,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="233" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:10">
       <c r="A233" s="1" t="s">
         <v>376</v>
       </c>
@@ -11122,12 +11132,12 @@
       <selection activeCell="E86" sqref="E86"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="3" max="3" width="19.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -11153,7 +11163,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8">
       <c r="A2" s="1" t="s">
         <v>96</v>
       </c>
@@ -11179,7 +11189,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8">
       <c r="A3" s="1" t="s">
         <v>107</v>
       </c>
@@ -11205,7 +11215,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8">
       <c r="A4" s="1" t="s">
         <v>107</v>
       </c>
@@ -11231,7 +11241,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8">
       <c r="A5" s="1" t="s">
         <v>107</v>
       </c>
@@ -11257,7 +11267,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8">
       <c r="A6" s="1" t="s">
         <v>115</v>
       </c>
@@ -11283,7 +11293,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8">
       <c r="A7" s="1" t="s">
         <v>115</v>
       </c>
@@ -11309,7 +11319,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8">
       <c r="A8" s="1" t="s">
         <v>115</v>
       </c>
@@ -11335,7 +11345,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8">
       <c r="A9" s="1" t="s">
         <v>115</v>
       </c>
@@ -11361,7 +11371,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8">
       <c r="A10" s="1" t="s">
         <v>123</v>
       </c>
@@ -11387,7 +11397,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8">
       <c r="A11" s="1" t="s">
         <v>123</v>
       </c>
@@ -11413,7 +11423,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8">
       <c r="A12" s="1" t="s">
         <v>123</v>
       </c>
@@ -11439,7 +11449,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8">
       <c r="A13" s="1" t="s">
         <v>123</v>
       </c>
@@ -11465,7 +11475,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8">
       <c r="A14" s="1" t="s">
         <v>123</v>
       </c>
@@ -11491,7 +11501,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8">
       <c r="A15" s="1" t="s">
         <v>128</v>
       </c>
@@ -11517,7 +11527,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8">
       <c r="A16" s="1" t="s">
         <v>128</v>
       </c>
@@ -11543,7 +11553,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8">
       <c r="A17" s="1" t="s">
         <v>128</v>
       </c>
@@ -11569,7 +11579,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8">
       <c r="A18" s="1" t="s">
         <v>128</v>
       </c>
@@ -11595,7 +11605,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8">
       <c r="A19" s="1" t="s">
         <v>128</v>
       </c>
@@ -11621,7 +11631,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8">
       <c r="A20" s="1" t="s">
         <v>138</v>
       </c>
@@ -11647,7 +11657,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8">
       <c r="A21" s="1" t="s">
         <v>138</v>
       </c>
@@ -11673,7 +11683,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8">
       <c r="A22" s="1" t="s">
         <v>138</v>
       </c>
@@ -11699,7 +11709,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8">
       <c r="A23" s="1" t="s">
         <v>138</v>
       </c>
@@ -11725,7 +11735,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8">
       <c r="A24" s="1" t="s">
         <v>138</v>
       </c>
@@ -11751,7 +11761,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8">
       <c r="A25" s="1" t="s">
         <v>144</v>
       </c>
@@ -11777,7 +11787,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8">
       <c r="A26" s="1" t="s">
         <v>144</v>
       </c>
@@ -11803,7 +11813,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8">
       <c r="A27" s="1" t="s">
         <v>144</v>
       </c>
@@ -11829,7 +11839,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8">
       <c r="A28" s="1" t="s">
         <v>144</v>
       </c>
@@ -11855,7 +11865,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8">
       <c r="A29" s="1" t="s">
         <v>149</v>
       </c>
@@ -11881,7 +11891,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8">
       <c r="A30" s="1" t="s">
         <v>149</v>
       </c>
@@ -11907,7 +11917,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8">
       <c r="A31" s="1" t="s">
         <v>149</v>
       </c>
@@ -11933,7 +11943,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8">
       <c r="A32" s="1" t="s">
         <v>149</v>
       </c>
@@ -11959,7 +11969,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8">
       <c r="A33" s="1" t="s">
         <v>158</v>
       </c>
@@ -11985,7 +11995,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8">
       <c r="A34" s="1" t="s">
         <v>158</v>
       </c>
@@ -12011,7 +12021,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8">
       <c r="A35" s="1" t="s">
         <v>158</v>
       </c>
@@ -12037,7 +12047,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8">
       <c r="A36" s="1" t="s">
         <v>158</v>
       </c>
@@ -12063,7 +12073,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8">
       <c r="A37" s="1" t="s">
         <v>163</v>
       </c>
@@ -12089,7 +12099,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8">
       <c r="A38" s="1" t="s">
         <v>163</v>
       </c>
@@ -12115,7 +12125,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8">
       <c r="A39" s="1" t="s">
         <v>163</v>
       </c>
@@ -12141,7 +12151,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8">
       <c r="A40" s="1" t="s">
         <v>163</v>
       </c>
@@ -12167,7 +12177,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8">
       <c r="A41" s="1" t="s">
         <v>169</v>
       </c>
@@ -12193,7 +12203,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8">
       <c r="A42" s="1" t="s">
         <v>187</v>
       </c>
@@ -12219,7 +12229,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8">
       <c r="A43" s="1" t="s">
         <v>204</v>
       </c>
@@ -12245,7 +12255,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8">
       <c r="A44" s="1" t="s">
         <v>221</v>
       </c>
@@ -12271,7 +12281,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8">
       <c r="A45" s="1" t="s">
         <v>239</v>
       </c>
@@ -12297,7 +12307,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8">
       <c r="A46" s="1" t="s">
         <v>257</v>
       </c>
@@ -12323,7 +12333,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8">
       <c r="A47" s="1" t="s">
         <v>271</v>
       </c>
@@ -12349,7 +12359,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8">
       <c r="A48" s="1" t="s">
         <v>271</v>
       </c>
@@ -12375,7 +12385,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8">
       <c r="A49" s="1" t="s">
         <v>271</v>
       </c>
@@ -12401,7 +12411,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8">
       <c r="A50" s="1" t="s">
         <v>271</v>
       </c>
@@ -12427,7 +12437,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8">
       <c r="A51" s="1" t="s">
         <v>280</v>
       </c>
@@ -12453,7 +12463,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8">
       <c r="A52" s="1" t="s">
         <v>280</v>
       </c>
@@ -12479,7 +12489,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8">
       <c r="A53" s="1" t="s">
         <v>280</v>
       </c>
@@ -12505,7 +12515,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8">
       <c r="A54" s="1" t="s">
         <v>280</v>
       </c>
@@ -12531,7 +12541,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8">
       <c r="A55" s="1" t="s">
         <v>280</v>
       </c>
@@ -12557,7 +12567,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8">
       <c r="A56" s="1" t="s">
         <v>286</v>
       </c>
@@ -12583,7 +12593,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8">
       <c r="A57" s="1" t="s">
         <v>286</v>
       </c>
@@ -12609,7 +12619,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8">
       <c r="A58" s="1" t="s">
         <v>286</v>
       </c>
@@ -12635,7 +12645,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8">
       <c r="A59" s="1" t="s">
         <v>286</v>
       </c>
@@ -12661,7 +12671,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8">
       <c r="A60" s="1" t="s">
         <v>291</v>
       </c>
@@ -12687,7 +12697,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8">
       <c r="A61" s="1" t="s">
         <v>291</v>
       </c>
@@ -12713,7 +12723,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8">
       <c r="A62" s="1" t="s">
         <v>291</v>
       </c>
@@ -12739,7 +12749,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8">
       <c r="A63" s="1" t="s">
         <v>299</v>
       </c>
@@ -12765,7 +12775,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8">
       <c r="A64" s="1" t="s">
         <v>299</v>
       </c>
@@ -12791,7 +12801,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8">
       <c r="A65" s="1" t="s">
         <v>299</v>
       </c>
@@ -12817,7 +12827,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8">
       <c r="A66" s="1" t="s">
         <v>304</v>
       </c>
@@ -12843,7 +12853,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8">
       <c r="A67" s="1" t="s">
         <v>304</v>
       </c>
@@ -12869,7 +12879,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8">
       <c r="A68" s="1" t="s">
         <v>304</v>
       </c>
@@ -12895,7 +12905,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8">
       <c r="A69" s="1" t="s">
         <v>309</v>
       </c>
@@ -12921,7 +12931,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8">
       <c r="A70" s="1" t="s">
         <v>309</v>
       </c>
@@ -12947,7 +12957,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8">
       <c r="A71" s="1" t="s">
         <v>309</v>
       </c>
@@ -12973,7 +12983,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8">
       <c r="A72" s="1" t="s">
         <v>309</v>
       </c>
@@ -12999,7 +13009,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8">
       <c r="A73" s="1" t="s">
         <v>318</v>
       </c>
@@ -13025,7 +13035,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8">
       <c r="A74" s="1" t="s">
         <v>318</v>
       </c>
@@ -13051,7 +13061,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8">
       <c r="A75" s="1" t="s">
         <v>318</v>
       </c>
@@ -13077,7 +13087,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8">
       <c r="A76" s="1" t="s">
         <v>318</v>
       </c>
@@ -13103,7 +13113,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8">
       <c r="A77" s="1" t="s">
         <v>328</v>
       </c>
@@ -13129,7 +13139,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8">
       <c r="A78" s="1" t="s">
         <v>346</v>
       </c>
@@ -13155,7 +13165,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8">
       <c r="A79" s="1" t="s">
         <v>352</v>
       </c>
@@ -13181,7 +13191,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8">
       <c r="A80" s="1" t="s">
         <v>358</v>
       </c>
@@ -13207,7 +13217,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8">
       <c r="A81" s="1" t="s">
         <v>364</v>
       </c>
@@ -13233,7 +13243,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8">
       <c r="A82" s="1" t="s">
         <v>370</v>
       </c>
@@ -13259,7 +13269,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8">
       <c r="A83" s="1" t="s">
         <v>376</v>
       </c>
@@ -13293,15 +13303,15 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:H54"/>
+  <dimension ref="A1:H58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="P45" sqref="P45"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="C57" sqref="C57:E58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -13327,7 +13337,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8">
       <c r="A2" s="1" t="s">
         <v>96</v>
       </c>
@@ -13353,7 +13363,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8">
       <c r="A3" s="1" t="s">
         <v>107</v>
       </c>
@@ -13379,7 +13389,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8">
       <c r="A4" s="1" t="s">
         <v>115</v>
       </c>
@@ -13405,7 +13415,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8">
       <c r="A5" s="1" t="s">
         <v>123</v>
       </c>
@@ -13431,7 +13441,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8">
       <c r="A6" s="1" t="s">
         <v>128</v>
       </c>
@@ -13457,7 +13467,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8">
       <c r="A7" s="1" t="s">
         <v>138</v>
       </c>
@@ -13483,7 +13493,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8">
       <c r="A8" s="1" t="s">
         <v>144</v>
       </c>
@@ -13509,7 +13519,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8">
       <c r="A9" s="1" t="s">
         <v>149</v>
       </c>
@@ -13535,7 +13545,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8">
       <c r="A10" s="1" t="s">
         <v>158</v>
       </c>
@@ -13561,7 +13571,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8">
       <c r="A11" s="1" t="s">
         <v>163</v>
       </c>
@@ -13587,7 +13597,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8">
       <c r="A12" s="1" t="s">
         <v>168</v>
       </c>
@@ -13613,7 +13623,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8">
       <c r="A13" s="1" t="s">
         <v>169</v>
       </c>
@@ -13639,7 +13649,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8">
       <c r="A14" s="1" t="s">
         <v>187</v>
       </c>
@@ -13665,7 +13675,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8">
       <c r="A15" s="1" t="s">
         <v>204</v>
       </c>
@@ -13691,7 +13701,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8">
       <c r="A16" s="1" t="s">
         <v>221</v>
       </c>
@@ -13717,7 +13727,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8">
       <c r="A17" s="1" t="s">
         <v>239</v>
       </c>
@@ -13743,7 +13753,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8">
       <c r="A18" s="1" t="s">
         <v>257</v>
       </c>
@@ -13769,7 +13779,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8">
       <c r="A19" s="1" t="s">
         <v>271</v>
       </c>
@@ -13795,7 +13805,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8">
       <c r="A20" s="1" t="s">
         <v>280</v>
       </c>
@@ -13821,7 +13831,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8">
       <c r="A21" s="1" t="s">
         <v>286</v>
       </c>
@@ -13847,7 +13857,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8">
       <c r="A22" s="1" t="s">
         <v>291</v>
       </c>
@@ -13873,7 +13883,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8">
       <c r="A23" s="1" t="s">
         <v>299</v>
       </c>
@@ -13899,7 +13909,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8">
       <c r="A24" s="1" t="s">
         <v>304</v>
       </c>
@@ -13925,7 +13935,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8">
       <c r="A25" s="1" t="s">
         <v>309</v>
       </c>
@@ -13951,7 +13961,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8">
       <c r="A26" s="1" t="s">
         <v>318</v>
       </c>
@@ -13977,7 +13987,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8">
       <c r="A27" s="1" t="s">
         <v>328</v>
       </c>
@@ -14003,7 +14013,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8">
       <c r="A28" s="1" t="s">
         <v>346</v>
       </c>
@@ -14029,7 +14039,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8">
       <c r="A29" s="1" t="s">
         <v>352</v>
       </c>
@@ -14055,7 +14065,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8">
       <c r="A30" s="1" t="s">
         <v>358</v>
       </c>
@@ -14081,7 +14091,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8">
       <c r="A31" s="1" t="s">
         <v>364</v>
       </c>
@@ -14107,7 +14117,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8">
       <c r="A32" s="1" t="s">
         <v>370</v>
       </c>
@@ -14133,7 +14143,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8">
       <c r="A33" s="1" t="s">
         <v>378</v>
       </c>
@@ -14159,7 +14169,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8">
       <c r="A34" s="1" t="s">
         <v>379</v>
       </c>
@@ -14185,7 +14195,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8">
       <c r="A35" s="1" t="s">
         <v>380</v>
       </c>
@@ -14211,7 +14221,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8">
       <c r="A36" s="1" t="s">
         <v>381</v>
       </c>
@@ -14237,7 +14247,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8">
       <c r="A37" s="1" t="s">
         <v>382</v>
       </c>
@@ -14263,7 +14273,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8">
       <c r="A38" s="1" t="s">
         <v>383</v>
       </c>
@@ -14289,7 +14299,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8">
       <c r="A39" s="1" t="s">
         <v>384</v>
       </c>
@@ -14315,7 +14325,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8">
       <c r="A40" s="1" t="s">
         <v>385</v>
       </c>
@@ -14341,7 +14351,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8">
       <c r="A41" s="1" t="s">
         <v>386</v>
       </c>
@@ -14367,7 +14377,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8">
       <c r="A42" s="1" t="s">
         <v>387</v>
       </c>
@@ -14393,7 +14403,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8">
       <c r="A43" s="1" t="s">
         <v>388</v>
       </c>
@@ -14419,7 +14429,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8">
       <c r="A44" s="1" t="s">
         <v>389</v>
       </c>
@@ -14445,7 +14455,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8">
       <c r="A45" s="1" t="s">
         <v>390</v>
       </c>
@@ -14471,7 +14481,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8">
       <c r="A46" s="1" t="s">
         <v>391</v>
       </c>
@@ -14497,7 +14507,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8">
       <c r="A47" s="1" t="s">
         <v>392</v>
       </c>
@@ -14523,7 +14533,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8">
       <c r="A48" s="1" t="s">
         <v>393</v>
       </c>
@@ -14549,7 +14559,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8">
       <c r="A49" s="1" t="s">
         <v>394</v>
       </c>
@@ -14575,7 +14585,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8">
       <c r="A50" s="1" t="s">
         <v>395</v>
       </c>
@@ -14601,7 +14611,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8">
       <c r="A51" s="1" t="s">
         <v>396</v>
       </c>
@@ -14627,7 +14637,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8">
       <c r="A52" s="1" t="s">
         <v>397</v>
       </c>
@@ -14653,7 +14663,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8">
       <c r="A53" s="1" t="s">
         <v>428</v>
       </c>
@@ -14679,7 +14689,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8">
       <c r="A54" s="1" t="s">
         <v>429</v>
       </c>
@@ -14702,6 +14712,110 @@
         <v>28</v>
       </c>
       <c r="H54" s="1">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8">
+      <c r="A55" s="1" t="s">
+        <v>430</v>
+      </c>
+      <c r="B55" s="1">
+        <v>0</v>
+      </c>
+      <c r="C55" s="1">
+        <v>-3591</v>
+      </c>
+      <c r="D55" s="1">
+        <v>-85</v>
+      </c>
+      <c r="E55" s="1">
+        <v>-3296</v>
+      </c>
+      <c r="F55" s="1">
+        <v>40</v>
+      </c>
+      <c r="G55" s="1">
+        <v>28</v>
+      </c>
+      <c r="H55" s="1">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8">
+      <c r="A56" s="1" t="s">
+        <v>431</v>
+      </c>
+      <c r="B56" s="1">
+        <v>0</v>
+      </c>
+      <c r="C56" s="1">
+        <v>-3591</v>
+      </c>
+      <c r="D56" s="1">
+        <v>-85</v>
+      </c>
+      <c r="E56" s="1">
+        <v>-3296</v>
+      </c>
+      <c r="F56" s="1">
+        <v>40</v>
+      </c>
+      <c r="G56" s="1">
+        <v>28</v>
+      </c>
+      <c r="H56" s="1">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8">
+      <c r="A57" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="B57" s="1">
+        <v>0</v>
+      </c>
+      <c r="C57" s="1">
+        <v>3205</v>
+      </c>
+      <c r="D57" s="1">
+        <v>292</v>
+      </c>
+      <c r="E57" s="1">
+        <v>3455</v>
+      </c>
+      <c r="F57" s="1">
+        <v>40</v>
+      </c>
+      <c r="G57" s="1">
+        <v>28</v>
+      </c>
+      <c r="H57" s="1">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8">
+      <c r="A58" s="1" t="s">
+        <v>433</v>
+      </c>
+      <c r="B58" s="1">
+        <v>0</v>
+      </c>
+      <c r="C58" s="1">
+        <v>3205</v>
+      </c>
+      <c r="D58" s="1">
+        <v>292</v>
+      </c>
+      <c r="E58" s="1">
+        <v>3455</v>
+      </c>
+      <c r="F58" s="1">
+        <v>40</v>
+      </c>
+      <c r="G58" s="1">
+        <v>28</v>
+      </c>
+      <c r="H58" s="1">
         <v>40</v>
       </c>
     </row>
@@ -14717,9 +14831,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>398</v>
       </c>
@@ -14742,7 +14856,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" s="1" t="s">
         <v>399</v>
       </c>
@@ -14765,7 +14879,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -14788,7 +14902,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7">
       <c r="A4" s="1">
         <v>51</v>
       </c>
@@ -14811,7 +14925,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7">
       <c r="A5" s="1">
         <v>101</v>
       </c>
@@ -14834,7 +14948,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7">
       <c r="A6" s="1">
         <v>151</v>
       </c>
@@ -14857,7 +14971,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7">
       <c r="A7" s="1">
         <v>201</v>
       </c>
@@ -14880,7 +14994,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7">
       <c r="A8" s="1">
         <v>251</v>
       </c>
@@ -14903,7 +15017,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7">
       <c r="A9" s="1">
         <v>46</v>
       </c>

</xml_diff>

<commit_message>
HQ Buffer all race
</commit_message>
<xml_diff>
--- a/gu_in/Map.edf/Sette.xlsx
+++ b/gu_in/Map.edf/Sette.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\emay.dev\Parser_1.0.2\Database\gu_in\Map.edf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6790F68C-605A-4533-A666-2F90D5328400}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02675A6F-3404-4883-B02F-F7D2330DB7C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5235" yWindow="1320" windowWidth="18480" windowHeight="11205" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -13306,7 +13306,7 @@
   <dimension ref="A1:H58"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="C57" sqref="C57:E58"/>
+      <selection activeCell="E57" sqref="C57:E58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -14775,13 +14775,13 @@
         <v>0</v>
       </c>
       <c r="C57" s="1">
-        <v>3205</v>
+        <v>3341</v>
       </c>
       <c r="D57" s="1">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="E57" s="1">
-        <v>3455</v>
+        <v>3109</v>
       </c>
       <c r="F57" s="1">
         <v>40</v>
@@ -14801,13 +14801,13 @@
         <v>0</v>
       </c>
       <c r="C58" s="1">
-        <v>3205</v>
+        <v>3341</v>
       </c>
       <c r="D58" s="1">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="E58" s="1">
-        <v>3455</v>
+        <v>3109</v>
       </c>
       <c r="F58" s="1">
         <v>40</v>

</xml_diff>